<commit_message>
GET STARTED BTN IS SOLO
</commit_message>
<xml_diff>
--- a/OOSA Survey Content - Temp Content v2.xlsx
+++ b/OOSA Survey Content - Temp Content v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike Steeze\Desktop\CPR\Oracle\2021\assess_tools\sec_tool--demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30890E8C-271E-47C5-9231-3D36EE656A82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1348AC69-B8A5-4B25-8818-AC3B0292B692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32040" yWindow="1350" windowWidth="22995" windowHeight="14070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exec Summaries" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>Introduction Paragraphs</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>Question Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score </t>
   </si>
   <si>
     <t>Score Weight</t>
@@ -449,6 +446,39 @@
 j. Failed to meet customer SLAs
 k. Lost customers</t>
   </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Cloud Service Types</t>
+  </si>
+  <si>
+    <t>Public Cloud Repository</t>
+  </si>
+  <si>
+    <t>Cloud Integrity</t>
+  </si>
+  <si>
+    <t>Data Leaks</t>
+  </si>
+  <si>
+    <t>Data Loss</t>
+  </si>
+  <si>
+    <t>Data Breach</t>
+  </si>
+  <si>
+    <t>Service Providers</t>
+  </si>
+  <si>
+    <t>Readiness</t>
+  </si>
+  <si>
+    <t>Security Comprehension</t>
+  </si>
+  <si>
+    <t>Personal Confedentiality</t>
+  </si>
 </sst>
 </file>
 
@@ -543,7 +573,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +601,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -924,6 +966,42 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -940,18 +1018,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="13" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2115,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2132,10 +2203,10 @@
   <sheetData>
     <row r="1" spans="1:256" ht="48.95" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -2394,10 +2465,10 @@
     </row>
     <row r="2" spans="1:256" ht="102" customHeight="1">
       <c r="A2" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
@@ -2425,11 +2496,11 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
@@ -2486,12 +2557,12 @@
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="54"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="75"/>
       <c r="F5" s="14"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -2515,13 +2586,13 @@
       <c r="Z5" s="7"/>
     </row>
     <row r="6" spans="1:256" ht="141.75" customHeight="1">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="54"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="75"/>
       <c r="F6" s="14"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -2548,12 +2619,12 @@
       <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="54"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="14"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -2577,13 +2648,13 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="1:256" ht="295.5" customHeight="1">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="54"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="75"/>
       <c r="F8" s="14"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -2610,12 +2681,12 @@
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="54"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="75"/>
       <c r="F9" s="14"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -2639,15 +2710,15 @@
       <c r="Z9" s="7"/>
     </row>
     <row r="10" spans="1:256" ht="195.75" customHeight="1">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59" t="s">
+      <c r="B10" s="78"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="54"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="14"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -2674,12 +2745,12 @@
       <c r="A11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="54"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="75"/>
       <c r="F11" s="14"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2703,13 +2774,13 @@
       <c r="Z11" s="7"/>
     </row>
     <row r="12" spans="1:256" ht="198" customHeight="1">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="54"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="75"/>
       <c r="F12" s="14"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -30456,8 +30527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV951"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" activeCellId="1" sqref="A8 B8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -30474,7 +30546,7 @@
   <sheetData>
     <row r="1" spans="1:256" s="43" customFormat="1" ht="24" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -30740,16 +30812,16 @@
         <v>17</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="25" t="s">
         <v>16</v>
@@ -30777,15 +30849,15 @@
       <c r="AB2" s="7"/>
     </row>
     <row r="3" spans="1:256" ht="84" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61" t="s">
-        <v>21</v>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
@@ -30813,15 +30885,15 @@
       <c r="AB3" s="7"/>
     </row>
     <row r="4" spans="1:256" ht="69.75" customHeight="1">
-      <c r="A4" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="61" t="s">
+      <c r="A4" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61" t="s">
-        <v>21</v>
+      <c r="B4" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="27"/>
@@ -30849,15 +30921,15 @@
       <c r="AB4" s="7"/>
     </row>
     <row r="5" spans="1:256" ht="196.35" customHeight="1">
-      <c r="A5" s="62" t="s">
-        <v>30</v>
+      <c r="A5" s="53" t="s">
+        <v>29</v>
       </c>
-      <c r="B5" s="62" t="s">
-        <v>45</v>
+      <c r="B5" s="53" t="s">
+        <v>44</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61" t="s">
-        <v>21</v>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
@@ -31113,15 +31185,15 @@
       <c r="IV5" s="31"/>
     </row>
     <row r="6" spans="1:256" ht="39.6" customHeight="1">
-      <c r="A6" s="62" t="s">
-        <v>31</v>
+      <c r="A6" s="53" t="s">
+        <v>30</v>
       </c>
-      <c r="B6" s="62" t="s">
-        <v>45</v>
+      <c r="B6" s="53" t="s">
+        <v>44</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61" t="s">
-        <v>21</v>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
@@ -31377,15 +31449,15 @@
       <c r="IV6" s="31"/>
     </row>
     <row r="7" spans="1:256" ht="155.44999999999999" customHeight="1">
-      <c r="A7" s="62" t="s">
-        <v>32</v>
+      <c r="A7" s="53" t="s">
+        <v>31</v>
       </c>
-      <c r="B7" s="61" t="s">
-        <v>45</v>
+      <c r="B7" s="52" t="s">
+        <v>44</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61" t="s">
-        <v>21</v>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
@@ -31641,15 +31713,15 @@
       <c r="IV7" s="31"/>
     </row>
     <row r="8" spans="1:256" ht="252" customHeight="1">
-      <c r="A8" s="62" t="s">
-        <v>33</v>
+      <c r="A8" s="53" t="s">
+        <v>32</v>
       </c>
-      <c r="B8" s="61" t="s">
-        <v>45</v>
+      <c r="B8" s="52" t="s">
+        <v>44</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61" t="s">
-        <v>21</v>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
@@ -31904,544 +31976,550 @@
       <c r="IU8" s="31"/>
       <c r="IV8" s="31"/>
     </row>
-    <row r="9" spans="1:256" ht="100.7" customHeight="1">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:256" s="71" customFormat="1" ht="100.7" customHeight="1">
+      <c r="A9" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="68"/>
+      <c r="S9" s="68"/>
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="68"/>
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="70"/>
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="70"/>
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="70"/>
+      <c r="AH9" s="70"/>
+      <c r="AI9" s="70"/>
+      <c r="AJ9" s="70"/>
+      <c r="AK9" s="70"/>
+      <c r="AL9" s="70"/>
+      <c r="AM9" s="70"/>
+      <c r="AN9" s="70"/>
+      <c r="AO9" s="70"/>
+      <c r="AP9" s="70"/>
+      <c r="AQ9" s="70"/>
+      <c r="AR9" s="70"/>
+      <c r="AS9" s="70"/>
+      <c r="AT9" s="70"/>
+      <c r="AU9" s="70"/>
+      <c r="AV9" s="70"/>
+      <c r="AW9" s="70"/>
+      <c r="AX9" s="70"/>
+      <c r="AY9" s="70"/>
+      <c r="AZ9" s="70"/>
+      <c r="BA9" s="70"/>
+      <c r="BB9" s="70"/>
+      <c r="BC9" s="70"/>
+      <c r="BD9" s="70"/>
+      <c r="BE9" s="70"/>
+      <c r="BF9" s="70"/>
+      <c r="BG9" s="70"/>
+      <c r="BH9" s="70"/>
+      <c r="BI9" s="70"/>
+      <c r="BJ9" s="70"/>
+      <c r="BK9" s="70"/>
+      <c r="BL9" s="70"/>
+      <c r="BM9" s="70"/>
+      <c r="BN9" s="70"/>
+      <c r="BO9" s="70"/>
+      <c r="BP9" s="70"/>
+      <c r="BQ9" s="70"/>
+      <c r="BR9" s="70"/>
+      <c r="BS9" s="70"/>
+      <c r="BT9" s="70"/>
+      <c r="BU9" s="70"/>
+      <c r="BV9" s="70"/>
+      <c r="BW9" s="70"/>
+      <c r="BX9" s="70"/>
+      <c r="BY9" s="70"/>
+      <c r="BZ9" s="70"/>
+      <c r="CA9" s="70"/>
+      <c r="CB9" s="70"/>
+      <c r="CC9" s="70"/>
+      <c r="CD9" s="70"/>
+      <c r="CE9" s="70"/>
+      <c r="CF9" s="70"/>
+      <c r="CG9" s="70"/>
+      <c r="CH9" s="70"/>
+      <c r="CI9" s="70"/>
+      <c r="CJ9" s="70"/>
+      <c r="CK9" s="70"/>
+      <c r="CL9" s="70"/>
+      <c r="CM9" s="70"/>
+      <c r="CN9" s="70"/>
+      <c r="CO9" s="70"/>
+      <c r="CP9" s="70"/>
+      <c r="CQ9" s="70"/>
+      <c r="CR9" s="70"/>
+      <c r="CS9" s="70"/>
+      <c r="CT9" s="70"/>
+      <c r="CU9" s="70"/>
+      <c r="CV9" s="70"/>
+      <c r="CW9" s="70"/>
+      <c r="CX9" s="70"/>
+      <c r="CY9" s="70"/>
+      <c r="CZ9" s="70"/>
+      <c r="DA9" s="70"/>
+      <c r="DB9" s="70"/>
+      <c r="DC9" s="70"/>
+      <c r="DD9" s="70"/>
+      <c r="DE9" s="70"/>
+      <c r="DF9" s="70"/>
+      <c r="DG9" s="70"/>
+      <c r="DH9" s="70"/>
+      <c r="DI9" s="70"/>
+      <c r="DJ9" s="70"/>
+      <c r="DK9" s="70"/>
+      <c r="DL9" s="70"/>
+      <c r="DM9" s="70"/>
+      <c r="DN9" s="70"/>
+      <c r="DO9" s="70"/>
+      <c r="DP9" s="70"/>
+      <c r="DQ9" s="70"/>
+      <c r="DR9" s="70"/>
+      <c r="DS9" s="70"/>
+      <c r="DT9" s="70"/>
+      <c r="DU9" s="70"/>
+      <c r="DV9" s="70"/>
+      <c r="DW9" s="70"/>
+      <c r="DX9" s="70"/>
+      <c r="DY9" s="70"/>
+      <c r="DZ9" s="70"/>
+      <c r="EA9" s="70"/>
+      <c r="EB9" s="70"/>
+      <c r="EC9" s="70"/>
+      <c r="ED9" s="70"/>
+      <c r="EE9" s="70"/>
+      <c r="EF9" s="70"/>
+      <c r="EG9" s="70"/>
+      <c r="EH9" s="70"/>
+      <c r="EI9" s="70"/>
+      <c r="EJ9" s="70"/>
+      <c r="EK9" s="70"/>
+      <c r="EL9" s="70"/>
+      <c r="EM9" s="70"/>
+      <c r="EN9" s="70"/>
+      <c r="EO9" s="70"/>
+      <c r="EP9" s="70"/>
+      <c r="EQ9" s="70"/>
+      <c r="ER9" s="70"/>
+      <c r="ES9" s="70"/>
+      <c r="ET9" s="70"/>
+      <c r="EU9" s="70"/>
+      <c r="EV9" s="70"/>
+      <c r="EW9" s="70"/>
+      <c r="EX9" s="70"/>
+      <c r="EY9" s="70"/>
+      <c r="EZ9" s="70"/>
+      <c r="FA9" s="70"/>
+      <c r="FB9" s="70"/>
+      <c r="FC9" s="70"/>
+      <c r="FD9" s="70"/>
+      <c r="FE9" s="70"/>
+      <c r="FF9" s="70"/>
+      <c r="FG9" s="70"/>
+      <c r="FH9" s="70"/>
+      <c r="FI9" s="70"/>
+      <c r="FJ9" s="70"/>
+      <c r="FK9" s="70"/>
+      <c r="FL9" s="70"/>
+      <c r="FM9" s="70"/>
+      <c r="FN9" s="70"/>
+      <c r="FO9" s="70"/>
+      <c r="FP9" s="70"/>
+      <c r="FQ9" s="70"/>
+      <c r="FR9" s="70"/>
+      <c r="FS9" s="70"/>
+      <c r="FT9" s="70"/>
+      <c r="FU9" s="70"/>
+      <c r="FV9" s="70"/>
+      <c r="FW9" s="70"/>
+      <c r="FX9" s="70"/>
+      <c r="FY9" s="70"/>
+      <c r="FZ9" s="70"/>
+      <c r="GA9" s="70"/>
+      <c r="GB9" s="70"/>
+      <c r="GC9" s="70"/>
+      <c r="GD9" s="70"/>
+      <c r="GE9" s="70"/>
+      <c r="GF9" s="70"/>
+      <c r="GG9" s="70"/>
+      <c r="GH9" s="70"/>
+      <c r="GI9" s="70"/>
+      <c r="GJ9" s="70"/>
+      <c r="GK9" s="70"/>
+      <c r="GL9" s="70"/>
+      <c r="GM9" s="70"/>
+      <c r="GN9" s="70"/>
+      <c r="GO9" s="70"/>
+      <c r="GP9" s="70"/>
+      <c r="GQ9" s="70"/>
+      <c r="GR9" s="70"/>
+      <c r="GS9" s="70"/>
+      <c r="GT9" s="70"/>
+      <c r="GU9" s="70"/>
+      <c r="GV9" s="70"/>
+      <c r="GW9" s="70"/>
+      <c r="GX9" s="70"/>
+      <c r="GY9" s="70"/>
+      <c r="GZ9" s="70"/>
+      <c r="HA9" s="70"/>
+      <c r="HB9" s="70"/>
+      <c r="HC9" s="70"/>
+      <c r="HD9" s="70"/>
+      <c r="HE9" s="70"/>
+      <c r="HF9" s="70"/>
+      <c r="HG9" s="70"/>
+      <c r="HH9" s="70"/>
+      <c r="HI9" s="70"/>
+      <c r="HJ9" s="70"/>
+      <c r="HK9" s="70"/>
+      <c r="HL9" s="70"/>
+      <c r="HM9" s="70"/>
+      <c r="HN9" s="70"/>
+      <c r="HO9" s="70"/>
+      <c r="HP9" s="70"/>
+      <c r="HQ9" s="70"/>
+      <c r="HR9" s="70"/>
+      <c r="HS9" s="70"/>
+      <c r="HT9" s="70"/>
+      <c r="HU9" s="70"/>
+      <c r="HV9" s="70"/>
+      <c r="HW9" s="70"/>
+      <c r="HX9" s="70"/>
+      <c r="HY9" s="70"/>
+      <c r="HZ9" s="70"/>
+      <c r="IA9" s="70"/>
+      <c r="IB9" s="70"/>
+      <c r="IC9" s="70"/>
+      <c r="ID9" s="70"/>
+      <c r="IE9" s="70"/>
+      <c r="IF9" s="70"/>
+      <c r="IG9" s="70"/>
+      <c r="IH9" s="70"/>
+      <c r="II9" s="70"/>
+      <c r="IJ9" s="70"/>
+      <c r="IK9" s="70"/>
+      <c r="IL9" s="70"/>
+      <c r="IM9" s="70"/>
+      <c r="IN9" s="70"/>
+      <c r="IO9" s="70"/>
+      <c r="IP9" s="70"/>
+      <c r="IQ9" s="70"/>
+      <c r="IR9" s="70"/>
+      <c r="IS9" s="70"/>
+      <c r="IT9" s="70"/>
+      <c r="IU9" s="70"/>
+      <c r="IV9" s="70"/>
+    </row>
+    <row r="10" spans="1:256" s="71" customFormat="1" ht="126.6" customHeight="1">
+      <c r="A10" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B10" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="27" t="s">
-        <v>21</v>
+      <c r="C10" s="64" t="s">
+        <v>49</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="32"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="32"/>
-      <c r="AA9" s="32"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="31"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
-      <c r="AF9" s="31"/>
-      <c r="AG9" s="31"/>
-      <c r="AH9" s="31"/>
-      <c r="AI9" s="31"/>
-      <c r="AJ9" s="31"/>
-      <c r="AK9" s="31"/>
-      <c r="AL9" s="31"/>
-      <c r="AM9" s="31"/>
-      <c r="AN9" s="31"/>
-      <c r="AO9" s="31"/>
-      <c r="AP9" s="31"/>
-      <c r="AQ9" s="31"/>
-      <c r="AR9" s="31"/>
-      <c r="AS9" s="31"/>
-      <c r="AT9" s="31"/>
-      <c r="AU9" s="31"/>
-      <c r="AV9" s="31"/>
-      <c r="AW9" s="31"/>
-      <c r="AX9" s="31"/>
-      <c r="AY9" s="31"/>
-      <c r="AZ9" s="31"/>
-      <c r="BA9" s="31"/>
-      <c r="BB9" s="31"/>
-      <c r="BC9" s="31"/>
-      <c r="BD9" s="31"/>
-      <c r="BE9" s="31"/>
-      <c r="BF9" s="31"/>
-      <c r="BG9" s="31"/>
-      <c r="BH9" s="31"/>
-      <c r="BI9" s="31"/>
-      <c r="BJ9" s="31"/>
-      <c r="BK9" s="31"/>
-      <c r="BL9" s="31"/>
-      <c r="BM9" s="31"/>
-      <c r="BN9" s="31"/>
-      <c r="BO9" s="31"/>
-      <c r="BP9" s="31"/>
-      <c r="BQ9" s="31"/>
-      <c r="BR9" s="31"/>
-      <c r="BS9" s="31"/>
-      <c r="BT9" s="31"/>
-      <c r="BU9" s="31"/>
-      <c r="BV9" s="31"/>
-      <c r="BW9" s="31"/>
-      <c r="BX9" s="31"/>
-      <c r="BY9" s="31"/>
-      <c r="BZ9" s="31"/>
-      <c r="CA9" s="31"/>
-      <c r="CB9" s="31"/>
-      <c r="CC9" s="31"/>
-      <c r="CD9" s="31"/>
-      <c r="CE9" s="31"/>
-      <c r="CF9" s="31"/>
-      <c r="CG9" s="31"/>
-      <c r="CH9" s="31"/>
-      <c r="CI9" s="31"/>
-      <c r="CJ9" s="31"/>
-      <c r="CK9" s="31"/>
-      <c r="CL9" s="31"/>
-      <c r="CM9" s="31"/>
-      <c r="CN9" s="31"/>
-      <c r="CO9" s="31"/>
-      <c r="CP9" s="31"/>
-      <c r="CQ9" s="31"/>
-      <c r="CR9" s="31"/>
-      <c r="CS9" s="31"/>
-      <c r="CT9" s="31"/>
-      <c r="CU9" s="31"/>
-      <c r="CV9" s="31"/>
-      <c r="CW9" s="31"/>
-      <c r="CX9" s="31"/>
-      <c r="CY9" s="31"/>
-      <c r="CZ9" s="31"/>
-      <c r="DA9" s="31"/>
-      <c r="DB9" s="31"/>
-      <c r="DC9" s="31"/>
-      <c r="DD9" s="31"/>
-      <c r="DE9" s="31"/>
-      <c r="DF9" s="31"/>
-      <c r="DG9" s="31"/>
-      <c r="DH9" s="31"/>
-      <c r="DI9" s="31"/>
-      <c r="DJ9" s="31"/>
-      <c r="DK9" s="31"/>
-      <c r="DL9" s="31"/>
-      <c r="DM9" s="31"/>
-      <c r="DN9" s="31"/>
-      <c r="DO9" s="31"/>
-      <c r="DP9" s="31"/>
-      <c r="DQ9" s="31"/>
-      <c r="DR9" s="31"/>
-      <c r="DS9" s="31"/>
-      <c r="DT9" s="31"/>
-      <c r="DU9" s="31"/>
-      <c r="DV9" s="31"/>
-      <c r="DW9" s="31"/>
-      <c r="DX9" s="31"/>
-      <c r="DY9" s="31"/>
-      <c r="DZ9" s="31"/>
-      <c r="EA9" s="31"/>
-      <c r="EB9" s="31"/>
-      <c r="EC9" s="31"/>
-      <c r="ED9" s="31"/>
-      <c r="EE9" s="31"/>
-      <c r="EF9" s="31"/>
-      <c r="EG9" s="31"/>
-      <c r="EH9" s="31"/>
-      <c r="EI9" s="31"/>
-      <c r="EJ9" s="31"/>
-      <c r="EK9" s="31"/>
-      <c r="EL9" s="31"/>
-      <c r="EM9" s="31"/>
-      <c r="EN9" s="31"/>
-      <c r="EO9" s="31"/>
-      <c r="EP9" s="31"/>
-      <c r="EQ9" s="31"/>
-      <c r="ER9" s="31"/>
-      <c r="ES9" s="31"/>
-      <c r="ET9" s="31"/>
-      <c r="EU9" s="31"/>
-      <c r="EV9" s="31"/>
-      <c r="EW9" s="31"/>
-      <c r="EX9" s="31"/>
-      <c r="EY9" s="31"/>
-      <c r="EZ9" s="31"/>
-      <c r="FA9" s="31"/>
-      <c r="FB9" s="31"/>
-      <c r="FC9" s="31"/>
-      <c r="FD9" s="31"/>
-      <c r="FE9" s="31"/>
-      <c r="FF9" s="31"/>
-      <c r="FG9" s="31"/>
-      <c r="FH9" s="31"/>
-      <c r="FI9" s="31"/>
-      <c r="FJ9" s="31"/>
-      <c r="FK9" s="31"/>
-      <c r="FL9" s="31"/>
-      <c r="FM9" s="31"/>
-      <c r="FN9" s="31"/>
-      <c r="FO9" s="31"/>
-      <c r="FP9" s="31"/>
-      <c r="FQ9" s="31"/>
-      <c r="FR9" s="31"/>
-      <c r="FS9" s="31"/>
-      <c r="FT9" s="31"/>
-      <c r="FU9" s="31"/>
-      <c r="FV9" s="31"/>
-      <c r="FW9" s="31"/>
-      <c r="FX9" s="31"/>
-      <c r="FY9" s="31"/>
-      <c r="FZ9" s="31"/>
-      <c r="GA9" s="31"/>
-      <c r="GB9" s="31"/>
-      <c r="GC9" s="31"/>
-      <c r="GD9" s="31"/>
-      <c r="GE9" s="31"/>
-      <c r="GF9" s="31"/>
-      <c r="GG9" s="31"/>
-      <c r="GH9" s="31"/>
-      <c r="GI9" s="31"/>
-      <c r="GJ9" s="31"/>
-      <c r="GK9" s="31"/>
-      <c r="GL9" s="31"/>
-      <c r="GM9" s="31"/>
-      <c r="GN9" s="31"/>
-      <c r="GO9" s="31"/>
-      <c r="GP9" s="31"/>
-      <c r="GQ9" s="31"/>
-      <c r="GR9" s="31"/>
-      <c r="GS9" s="31"/>
-      <c r="GT9" s="31"/>
-      <c r="GU9" s="31"/>
-      <c r="GV9" s="31"/>
-      <c r="GW9" s="31"/>
-      <c r="GX9" s="31"/>
-      <c r="GY9" s="31"/>
-      <c r="GZ9" s="31"/>
-      <c r="HA9" s="31"/>
-      <c r="HB9" s="31"/>
-      <c r="HC9" s="31"/>
-      <c r="HD9" s="31"/>
-      <c r="HE9" s="31"/>
-      <c r="HF9" s="31"/>
-      <c r="HG9" s="31"/>
-      <c r="HH9" s="31"/>
-      <c r="HI9" s="31"/>
-      <c r="HJ9" s="31"/>
-      <c r="HK9" s="31"/>
-      <c r="HL9" s="31"/>
-      <c r="HM9" s="31"/>
-      <c r="HN9" s="31"/>
-      <c r="HO9" s="31"/>
-      <c r="HP9" s="31"/>
-      <c r="HQ9" s="31"/>
-      <c r="HR9" s="31"/>
-      <c r="HS9" s="31"/>
-      <c r="HT9" s="31"/>
-      <c r="HU9" s="31"/>
-      <c r="HV9" s="31"/>
-      <c r="HW9" s="31"/>
-      <c r="HX9" s="31"/>
-      <c r="HY9" s="31"/>
-      <c r="HZ9" s="31"/>
-      <c r="IA9" s="31"/>
-      <c r="IB9" s="31"/>
-      <c r="IC9" s="31"/>
-      <c r="ID9" s="31"/>
-      <c r="IE9" s="31"/>
-      <c r="IF9" s="31"/>
-      <c r="IG9" s="31"/>
-      <c r="IH9" s="31"/>
-      <c r="II9" s="31"/>
-      <c r="IJ9" s="31"/>
-      <c r="IK9" s="31"/>
-      <c r="IL9" s="31"/>
-      <c r="IM9" s="31"/>
-      <c r="IN9" s="31"/>
-      <c r="IO9" s="31"/>
-      <c r="IP9" s="31"/>
-      <c r="IQ9" s="31"/>
-      <c r="IR9" s="31"/>
-      <c r="IS9" s="31"/>
-      <c r="IT9" s="31"/>
-      <c r="IU9" s="31"/>
-      <c r="IV9" s="31"/>
-    </row>
-    <row r="10" spans="1:256" ht="126.6" customHeight="1">
-      <c r="A10" s="50" t="s">
+      <c r="D10" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="68"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="70"/>
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="70"/>
+      <c r="AF10" s="70"/>
+      <c r="AG10" s="70"/>
+      <c r="AH10" s="70"/>
+      <c r="AI10" s="70"/>
+      <c r="AJ10" s="70"/>
+      <c r="AK10" s="70"/>
+      <c r="AL10" s="70"/>
+      <c r="AM10" s="70"/>
+      <c r="AN10" s="70"/>
+      <c r="AO10" s="70"/>
+      <c r="AP10" s="70"/>
+      <c r="AQ10" s="70"/>
+      <c r="AR10" s="70"/>
+      <c r="AS10" s="70"/>
+      <c r="AT10" s="70"/>
+      <c r="AU10" s="70"/>
+      <c r="AV10" s="70"/>
+      <c r="AW10" s="70"/>
+      <c r="AX10" s="70"/>
+      <c r="AY10" s="70"/>
+      <c r="AZ10" s="70"/>
+      <c r="BA10" s="70"/>
+      <c r="BB10" s="70"/>
+      <c r="BC10" s="70"/>
+      <c r="BD10" s="70"/>
+      <c r="BE10" s="70"/>
+      <c r="BF10" s="70"/>
+      <c r="BG10" s="70"/>
+      <c r="BH10" s="70"/>
+      <c r="BI10" s="70"/>
+      <c r="BJ10" s="70"/>
+      <c r="BK10" s="70"/>
+      <c r="BL10" s="70"/>
+      <c r="BM10" s="70"/>
+      <c r="BN10" s="70"/>
+      <c r="BO10" s="70"/>
+      <c r="BP10" s="70"/>
+      <c r="BQ10" s="70"/>
+      <c r="BR10" s="70"/>
+      <c r="BS10" s="70"/>
+      <c r="BT10" s="70"/>
+      <c r="BU10" s="70"/>
+      <c r="BV10" s="70"/>
+      <c r="BW10" s="70"/>
+      <c r="BX10" s="70"/>
+      <c r="BY10" s="70"/>
+      <c r="BZ10" s="70"/>
+      <c r="CA10" s="70"/>
+      <c r="CB10" s="70"/>
+      <c r="CC10" s="70"/>
+      <c r="CD10" s="70"/>
+      <c r="CE10" s="70"/>
+      <c r="CF10" s="70"/>
+      <c r="CG10" s="70"/>
+      <c r="CH10" s="70"/>
+      <c r="CI10" s="70"/>
+      <c r="CJ10" s="70"/>
+      <c r="CK10" s="70"/>
+      <c r="CL10" s="70"/>
+      <c r="CM10" s="70"/>
+      <c r="CN10" s="70"/>
+      <c r="CO10" s="70"/>
+      <c r="CP10" s="70"/>
+      <c r="CQ10" s="70"/>
+      <c r="CR10" s="70"/>
+      <c r="CS10" s="70"/>
+      <c r="CT10" s="70"/>
+      <c r="CU10" s="70"/>
+      <c r="CV10" s="70"/>
+      <c r="CW10" s="70"/>
+      <c r="CX10" s="70"/>
+      <c r="CY10" s="70"/>
+      <c r="CZ10" s="70"/>
+      <c r="DA10" s="70"/>
+      <c r="DB10" s="70"/>
+      <c r="DC10" s="70"/>
+      <c r="DD10" s="70"/>
+      <c r="DE10" s="70"/>
+      <c r="DF10" s="70"/>
+      <c r="DG10" s="70"/>
+      <c r="DH10" s="70"/>
+      <c r="DI10" s="70"/>
+      <c r="DJ10" s="70"/>
+      <c r="DK10" s="70"/>
+      <c r="DL10" s="70"/>
+      <c r="DM10" s="70"/>
+      <c r="DN10" s="70"/>
+      <c r="DO10" s="70"/>
+      <c r="DP10" s="70"/>
+      <c r="DQ10" s="70"/>
+      <c r="DR10" s="70"/>
+      <c r="DS10" s="70"/>
+      <c r="DT10" s="70"/>
+      <c r="DU10" s="70"/>
+      <c r="DV10" s="70"/>
+      <c r="DW10" s="70"/>
+      <c r="DX10" s="70"/>
+      <c r="DY10" s="70"/>
+      <c r="DZ10" s="70"/>
+      <c r="EA10" s="70"/>
+      <c r="EB10" s="70"/>
+      <c r="EC10" s="70"/>
+      <c r="ED10" s="70"/>
+      <c r="EE10" s="70"/>
+      <c r="EF10" s="70"/>
+      <c r="EG10" s="70"/>
+      <c r="EH10" s="70"/>
+      <c r="EI10" s="70"/>
+      <c r="EJ10" s="70"/>
+      <c r="EK10" s="70"/>
+      <c r="EL10" s="70"/>
+      <c r="EM10" s="70"/>
+      <c r="EN10" s="70"/>
+      <c r="EO10" s="70"/>
+      <c r="EP10" s="70"/>
+      <c r="EQ10" s="70"/>
+      <c r="ER10" s="70"/>
+      <c r="ES10" s="70"/>
+      <c r="ET10" s="70"/>
+      <c r="EU10" s="70"/>
+      <c r="EV10" s="70"/>
+      <c r="EW10" s="70"/>
+      <c r="EX10" s="70"/>
+      <c r="EY10" s="70"/>
+      <c r="EZ10" s="70"/>
+      <c r="FA10" s="70"/>
+      <c r="FB10" s="70"/>
+      <c r="FC10" s="70"/>
+      <c r="FD10" s="70"/>
+      <c r="FE10" s="70"/>
+      <c r="FF10" s="70"/>
+      <c r="FG10" s="70"/>
+      <c r="FH10" s="70"/>
+      <c r="FI10" s="70"/>
+      <c r="FJ10" s="70"/>
+      <c r="FK10" s="70"/>
+      <c r="FL10" s="70"/>
+      <c r="FM10" s="70"/>
+      <c r="FN10" s="70"/>
+      <c r="FO10" s="70"/>
+      <c r="FP10" s="70"/>
+      <c r="FQ10" s="70"/>
+      <c r="FR10" s="70"/>
+      <c r="FS10" s="70"/>
+      <c r="FT10" s="70"/>
+      <c r="FU10" s="70"/>
+      <c r="FV10" s="70"/>
+      <c r="FW10" s="70"/>
+      <c r="FX10" s="70"/>
+      <c r="FY10" s="70"/>
+      <c r="FZ10" s="70"/>
+      <c r="GA10" s="70"/>
+      <c r="GB10" s="70"/>
+      <c r="GC10" s="70"/>
+      <c r="GD10" s="70"/>
+      <c r="GE10" s="70"/>
+      <c r="GF10" s="70"/>
+      <c r="GG10" s="70"/>
+      <c r="GH10" s="70"/>
+      <c r="GI10" s="70"/>
+      <c r="GJ10" s="70"/>
+      <c r="GK10" s="70"/>
+      <c r="GL10" s="70"/>
+      <c r="GM10" s="70"/>
+      <c r="GN10" s="70"/>
+      <c r="GO10" s="70"/>
+      <c r="GP10" s="70"/>
+      <c r="GQ10" s="70"/>
+      <c r="GR10" s="70"/>
+      <c r="GS10" s="70"/>
+      <c r="GT10" s="70"/>
+      <c r="GU10" s="70"/>
+      <c r="GV10" s="70"/>
+      <c r="GW10" s="70"/>
+      <c r="GX10" s="70"/>
+      <c r="GY10" s="70"/>
+      <c r="GZ10" s="70"/>
+      <c r="HA10" s="70"/>
+      <c r="HB10" s="70"/>
+      <c r="HC10" s="70"/>
+      <c r="HD10" s="70"/>
+      <c r="HE10" s="70"/>
+      <c r="HF10" s="70"/>
+      <c r="HG10" s="70"/>
+      <c r="HH10" s="70"/>
+      <c r="HI10" s="70"/>
+      <c r="HJ10" s="70"/>
+      <c r="HK10" s="70"/>
+      <c r="HL10" s="70"/>
+      <c r="HM10" s="70"/>
+      <c r="HN10" s="70"/>
+      <c r="HO10" s="70"/>
+      <c r="HP10" s="70"/>
+      <c r="HQ10" s="70"/>
+      <c r="HR10" s="70"/>
+      <c r="HS10" s="70"/>
+      <c r="HT10" s="70"/>
+      <c r="HU10" s="70"/>
+      <c r="HV10" s="70"/>
+      <c r="HW10" s="70"/>
+      <c r="HX10" s="70"/>
+      <c r="HY10" s="70"/>
+      <c r="HZ10" s="70"/>
+      <c r="IA10" s="70"/>
+      <c r="IB10" s="70"/>
+      <c r="IC10" s="70"/>
+      <c r="ID10" s="70"/>
+      <c r="IE10" s="70"/>
+      <c r="IF10" s="70"/>
+      <c r="IG10" s="70"/>
+      <c r="IH10" s="70"/>
+      <c r="II10" s="70"/>
+      <c r="IJ10" s="70"/>
+      <c r="IK10" s="70"/>
+      <c r="IL10" s="70"/>
+      <c r="IM10" s="70"/>
+      <c r="IN10" s="70"/>
+      <c r="IO10" s="70"/>
+      <c r="IP10" s="70"/>
+      <c r="IQ10" s="70"/>
+      <c r="IR10" s="70"/>
+      <c r="IS10" s="70"/>
+      <c r="IT10" s="70"/>
+      <c r="IU10" s="70"/>
+      <c r="IV10" s="70"/>
+    </row>
+    <row r="11" spans="1:256" ht="201" customHeight="1">
+      <c r="A11" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>45</v>
+      <c r="B11" s="27" t="s">
+        <v>44</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="27" t="s">
-        <v>21</v>
+      <c r="C11" s="27" t="s">
+        <v>50</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="31"/>
-      <c r="AD10" s="31"/>
-      <c r="AE10" s="31"/>
-      <c r="AF10" s="31"/>
-      <c r="AG10" s="31"/>
-      <c r="AH10" s="31"/>
-      <c r="AI10" s="31"/>
-      <c r="AJ10" s="31"/>
-      <c r="AK10" s="31"/>
-      <c r="AL10" s="31"/>
-      <c r="AM10" s="31"/>
-      <c r="AN10" s="31"/>
-      <c r="AO10" s="31"/>
-      <c r="AP10" s="31"/>
-      <c r="AQ10" s="31"/>
-      <c r="AR10" s="31"/>
-      <c r="AS10" s="31"/>
-      <c r="AT10" s="31"/>
-      <c r="AU10" s="31"/>
-      <c r="AV10" s="31"/>
-      <c r="AW10" s="31"/>
-      <c r="AX10" s="31"/>
-      <c r="AY10" s="31"/>
-      <c r="AZ10" s="31"/>
-      <c r="BA10" s="31"/>
-      <c r="BB10" s="31"/>
-      <c r="BC10" s="31"/>
-      <c r="BD10" s="31"/>
-      <c r="BE10" s="31"/>
-      <c r="BF10" s="31"/>
-      <c r="BG10" s="31"/>
-      <c r="BH10" s="31"/>
-      <c r="BI10" s="31"/>
-      <c r="BJ10" s="31"/>
-      <c r="BK10" s="31"/>
-      <c r="BL10" s="31"/>
-      <c r="BM10" s="31"/>
-      <c r="BN10" s="31"/>
-      <c r="BO10" s="31"/>
-      <c r="BP10" s="31"/>
-      <c r="BQ10" s="31"/>
-      <c r="BR10" s="31"/>
-      <c r="BS10" s="31"/>
-      <c r="BT10" s="31"/>
-      <c r="BU10" s="31"/>
-      <c r="BV10" s="31"/>
-      <c r="BW10" s="31"/>
-      <c r="BX10" s="31"/>
-      <c r="BY10" s="31"/>
-      <c r="BZ10" s="31"/>
-      <c r="CA10" s="31"/>
-      <c r="CB10" s="31"/>
-      <c r="CC10" s="31"/>
-      <c r="CD10" s="31"/>
-      <c r="CE10" s="31"/>
-      <c r="CF10" s="31"/>
-      <c r="CG10" s="31"/>
-      <c r="CH10" s="31"/>
-      <c r="CI10" s="31"/>
-      <c r="CJ10" s="31"/>
-      <c r="CK10" s="31"/>
-      <c r="CL10" s="31"/>
-      <c r="CM10" s="31"/>
-      <c r="CN10" s="31"/>
-      <c r="CO10" s="31"/>
-      <c r="CP10" s="31"/>
-      <c r="CQ10" s="31"/>
-      <c r="CR10" s="31"/>
-      <c r="CS10" s="31"/>
-      <c r="CT10" s="31"/>
-      <c r="CU10" s="31"/>
-      <c r="CV10" s="31"/>
-      <c r="CW10" s="31"/>
-      <c r="CX10" s="31"/>
-      <c r="CY10" s="31"/>
-      <c r="CZ10" s="31"/>
-      <c r="DA10" s="31"/>
-      <c r="DB10" s="31"/>
-      <c r="DC10" s="31"/>
-      <c r="DD10" s="31"/>
-      <c r="DE10" s="31"/>
-      <c r="DF10" s="31"/>
-      <c r="DG10" s="31"/>
-      <c r="DH10" s="31"/>
-      <c r="DI10" s="31"/>
-      <c r="DJ10" s="31"/>
-      <c r="DK10" s="31"/>
-      <c r="DL10" s="31"/>
-      <c r="DM10" s="31"/>
-      <c r="DN10" s="31"/>
-      <c r="DO10" s="31"/>
-      <c r="DP10" s="31"/>
-      <c r="DQ10" s="31"/>
-      <c r="DR10" s="31"/>
-      <c r="DS10" s="31"/>
-      <c r="DT10" s="31"/>
-      <c r="DU10" s="31"/>
-      <c r="DV10" s="31"/>
-      <c r="DW10" s="31"/>
-      <c r="DX10" s="31"/>
-      <c r="DY10" s="31"/>
-      <c r="DZ10" s="31"/>
-      <c r="EA10" s="31"/>
-      <c r="EB10" s="31"/>
-      <c r="EC10" s="31"/>
-      <c r="ED10" s="31"/>
-      <c r="EE10" s="31"/>
-      <c r="EF10" s="31"/>
-      <c r="EG10" s="31"/>
-      <c r="EH10" s="31"/>
-      <c r="EI10" s="31"/>
-      <c r="EJ10" s="31"/>
-      <c r="EK10" s="31"/>
-      <c r="EL10" s="31"/>
-      <c r="EM10" s="31"/>
-      <c r="EN10" s="31"/>
-      <c r="EO10" s="31"/>
-      <c r="EP10" s="31"/>
-      <c r="EQ10" s="31"/>
-      <c r="ER10" s="31"/>
-      <c r="ES10" s="31"/>
-      <c r="ET10" s="31"/>
-      <c r="EU10" s="31"/>
-      <c r="EV10" s="31"/>
-      <c r="EW10" s="31"/>
-      <c r="EX10" s="31"/>
-      <c r="EY10" s="31"/>
-      <c r="EZ10" s="31"/>
-      <c r="FA10" s="31"/>
-      <c r="FB10" s="31"/>
-      <c r="FC10" s="31"/>
-      <c r="FD10" s="31"/>
-      <c r="FE10" s="31"/>
-      <c r="FF10" s="31"/>
-      <c r="FG10" s="31"/>
-      <c r="FH10" s="31"/>
-      <c r="FI10" s="31"/>
-      <c r="FJ10" s="31"/>
-      <c r="FK10" s="31"/>
-      <c r="FL10" s="31"/>
-      <c r="FM10" s="31"/>
-      <c r="FN10" s="31"/>
-      <c r="FO10" s="31"/>
-      <c r="FP10" s="31"/>
-      <c r="FQ10" s="31"/>
-      <c r="FR10" s="31"/>
-      <c r="FS10" s="31"/>
-      <c r="FT10" s="31"/>
-      <c r="FU10" s="31"/>
-      <c r="FV10" s="31"/>
-      <c r="FW10" s="31"/>
-      <c r="FX10" s="31"/>
-      <c r="FY10" s="31"/>
-      <c r="FZ10" s="31"/>
-      <c r="GA10" s="31"/>
-      <c r="GB10" s="31"/>
-      <c r="GC10" s="31"/>
-      <c r="GD10" s="31"/>
-      <c r="GE10" s="31"/>
-      <c r="GF10" s="31"/>
-      <c r="GG10" s="31"/>
-      <c r="GH10" s="31"/>
-      <c r="GI10" s="31"/>
-      <c r="GJ10" s="31"/>
-      <c r="GK10" s="31"/>
-      <c r="GL10" s="31"/>
-      <c r="GM10" s="31"/>
-      <c r="GN10" s="31"/>
-      <c r="GO10" s="31"/>
-      <c r="GP10" s="31"/>
-      <c r="GQ10" s="31"/>
-      <c r="GR10" s="31"/>
-      <c r="GS10" s="31"/>
-      <c r="GT10" s="31"/>
-      <c r="GU10" s="31"/>
-      <c r="GV10" s="31"/>
-      <c r="GW10" s="31"/>
-      <c r="GX10" s="31"/>
-      <c r="GY10" s="31"/>
-      <c r="GZ10" s="31"/>
-      <c r="HA10" s="31"/>
-      <c r="HB10" s="31"/>
-      <c r="HC10" s="31"/>
-      <c r="HD10" s="31"/>
-      <c r="HE10" s="31"/>
-      <c r="HF10" s="31"/>
-      <c r="HG10" s="31"/>
-      <c r="HH10" s="31"/>
-      <c r="HI10" s="31"/>
-      <c r="HJ10" s="31"/>
-      <c r="HK10" s="31"/>
-      <c r="HL10" s="31"/>
-      <c r="HM10" s="31"/>
-      <c r="HN10" s="31"/>
-      <c r="HO10" s="31"/>
-      <c r="HP10" s="31"/>
-      <c r="HQ10" s="31"/>
-      <c r="HR10" s="31"/>
-      <c r="HS10" s="31"/>
-      <c r="HT10" s="31"/>
-      <c r="HU10" s="31"/>
-      <c r="HV10" s="31"/>
-      <c r="HW10" s="31"/>
-      <c r="HX10" s="31"/>
-      <c r="HY10" s="31"/>
-      <c r="HZ10" s="31"/>
-      <c r="IA10" s="31"/>
-      <c r="IB10" s="31"/>
-      <c r="IC10" s="31"/>
-      <c r="ID10" s="31"/>
-      <c r="IE10" s="31"/>
-      <c r="IF10" s="31"/>
-      <c r="IG10" s="31"/>
-      <c r="IH10" s="31"/>
-      <c r="II10" s="31"/>
-      <c r="IJ10" s="31"/>
-      <c r="IK10" s="31"/>
-      <c r="IL10" s="31"/>
-      <c r="IM10" s="31"/>
-      <c r="IN10" s="31"/>
-      <c r="IO10" s="31"/>
-      <c r="IP10" s="31"/>
-      <c r="IQ10" s="31"/>
-      <c r="IR10" s="31"/>
-      <c r="IS10" s="31"/>
-      <c r="IT10" s="31"/>
-      <c r="IU10" s="31"/>
-      <c r="IV10" s="31"/>
-    </row>
-    <row r="11" spans="1:256" ht="201" customHeight="1">
-      <c r="A11" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="50"/>
       <c r="D11" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
@@ -32698,14 +32776,16 @@
     </row>
     <row r="12" spans="1:256" ht="141" customHeight="1">
       <c r="A12" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
-      <c r="C12" s="50"/>
+      <c r="C12" s="27" t="s">
+        <v>51</v>
+      </c>
       <c r="D12" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
@@ -32962,14 +33042,16 @@
     </row>
     <row r="13" spans="1:256" ht="249.6" customHeight="1">
       <c r="A13" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
-      <c r="C13" s="50"/>
+      <c r="C13" s="27" t="s">
+        <v>52</v>
+      </c>
       <c r="D13" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -33224,1397 +33306,1863 @@
       <c r="IU13" s="31"/>
       <c r="IV13" s="31"/>
     </row>
-    <row r="14" spans="1:256" ht="114" customHeight="1">
-      <c r="A14" s="50" t="s">
+    <row r="14" spans="1:256" s="71" customFormat="1" ht="114" customHeight="1">
+      <c r="A14" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="68"/>
+      <c r="P14" s="68"/>
+      <c r="Q14" s="68"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="68"/>
+      <c r="T14" s="68"/>
+      <c r="U14" s="68"/>
+      <c r="V14" s="68"/>
+      <c r="W14" s="68"/>
+      <c r="X14" s="68"/>
+      <c r="Y14" s="68"/>
+      <c r="Z14" s="68"/>
+      <c r="AA14" s="68"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="70"/>
+      <c r="AD14" s="70"/>
+      <c r="AE14" s="70"/>
+      <c r="AF14" s="70"/>
+      <c r="AG14" s="70"/>
+      <c r="AH14" s="70"/>
+      <c r="AI14" s="70"/>
+      <c r="AJ14" s="70"/>
+      <c r="AK14" s="70"/>
+      <c r="AL14" s="70"/>
+      <c r="AM14" s="70"/>
+      <c r="AN14" s="70"/>
+      <c r="AO14" s="70"/>
+      <c r="AP14" s="70"/>
+      <c r="AQ14" s="70"/>
+      <c r="AR14" s="70"/>
+      <c r="AS14" s="70"/>
+      <c r="AT14" s="70"/>
+      <c r="AU14" s="70"/>
+      <c r="AV14" s="70"/>
+      <c r="AW14" s="70"/>
+      <c r="AX14" s="70"/>
+      <c r="AY14" s="70"/>
+      <c r="AZ14" s="70"/>
+      <c r="BA14" s="70"/>
+      <c r="BB14" s="70"/>
+      <c r="BC14" s="70"/>
+      <c r="BD14" s="70"/>
+      <c r="BE14" s="70"/>
+      <c r="BF14" s="70"/>
+      <c r="BG14" s="70"/>
+      <c r="BH14" s="70"/>
+      <c r="BI14" s="70"/>
+      <c r="BJ14" s="70"/>
+      <c r="BK14" s="70"/>
+      <c r="BL14" s="70"/>
+      <c r="BM14" s="70"/>
+      <c r="BN14" s="70"/>
+      <c r="BO14" s="70"/>
+      <c r="BP14" s="70"/>
+      <c r="BQ14" s="70"/>
+      <c r="BR14" s="70"/>
+      <c r="BS14" s="70"/>
+      <c r="BT14" s="70"/>
+      <c r="BU14" s="70"/>
+      <c r="BV14" s="70"/>
+      <c r="BW14" s="70"/>
+      <c r="BX14" s="70"/>
+      <c r="BY14" s="70"/>
+      <c r="BZ14" s="70"/>
+      <c r="CA14" s="70"/>
+      <c r="CB14" s="70"/>
+      <c r="CC14" s="70"/>
+      <c r="CD14" s="70"/>
+      <c r="CE14" s="70"/>
+      <c r="CF14" s="70"/>
+      <c r="CG14" s="70"/>
+      <c r="CH14" s="70"/>
+      <c r="CI14" s="70"/>
+      <c r="CJ14" s="70"/>
+      <c r="CK14" s="70"/>
+      <c r="CL14" s="70"/>
+      <c r="CM14" s="70"/>
+      <c r="CN14" s="70"/>
+      <c r="CO14" s="70"/>
+      <c r="CP14" s="70"/>
+      <c r="CQ14" s="70"/>
+      <c r="CR14" s="70"/>
+      <c r="CS14" s="70"/>
+      <c r="CT14" s="70"/>
+      <c r="CU14" s="70"/>
+      <c r="CV14" s="70"/>
+      <c r="CW14" s="70"/>
+      <c r="CX14" s="70"/>
+      <c r="CY14" s="70"/>
+      <c r="CZ14" s="70"/>
+      <c r="DA14" s="70"/>
+      <c r="DB14" s="70"/>
+      <c r="DC14" s="70"/>
+      <c r="DD14" s="70"/>
+      <c r="DE14" s="70"/>
+      <c r="DF14" s="70"/>
+      <c r="DG14" s="70"/>
+      <c r="DH14" s="70"/>
+      <c r="DI14" s="70"/>
+      <c r="DJ14" s="70"/>
+      <c r="DK14" s="70"/>
+      <c r="DL14" s="70"/>
+      <c r="DM14" s="70"/>
+      <c r="DN14" s="70"/>
+      <c r="DO14" s="70"/>
+      <c r="DP14" s="70"/>
+      <c r="DQ14" s="70"/>
+      <c r="DR14" s="70"/>
+      <c r="DS14" s="70"/>
+      <c r="DT14" s="70"/>
+      <c r="DU14" s="70"/>
+      <c r="DV14" s="70"/>
+      <c r="DW14" s="70"/>
+      <c r="DX14" s="70"/>
+      <c r="DY14" s="70"/>
+      <c r="DZ14" s="70"/>
+      <c r="EA14" s="70"/>
+      <c r="EB14" s="70"/>
+      <c r="EC14" s="70"/>
+      <c r="ED14" s="70"/>
+      <c r="EE14" s="70"/>
+      <c r="EF14" s="70"/>
+      <c r="EG14" s="70"/>
+      <c r="EH14" s="70"/>
+      <c r="EI14" s="70"/>
+      <c r="EJ14" s="70"/>
+      <c r="EK14" s="70"/>
+      <c r="EL14" s="70"/>
+      <c r="EM14" s="70"/>
+      <c r="EN14" s="70"/>
+      <c r="EO14" s="70"/>
+      <c r="EP14" s="70"/>
+      <c r="EQ14" s="70"/>
+      <c r="ER14" s="70"/>
+      <c r="ES14" s="70"/>
+      <c r="ET14" s="70"/>
+      <c r="EU14" s="70"/>
+      <c r="EV14" s="70"/>
+      <c r="EW14" s="70"/>
+      <c r="EX14" s="70"/>
+      <c r="EY14" s="70"/>
+      <c r="EZ14" s="70"/>
+      <c r="FA14" s="70"/>
+      <c r="FB14" s="70"/>
+      <c r="FC14" s="70"/>
+      <c r="FD14" s="70"/>
+      <c r="FE14" s="70"/>
+      <c r="FF14" s="70"/>
+      <c r="FG14" s="70"/>
+      <c r="FH14" s="70"/>
+      <c r="FI14" s="70"/>
+      <c r="FJ14" s="70"/>
+      <c r="FK14" s="70"/>
+      <c r="FL14" s="70"/>
+      <c r="FM14" s="70"/>
+      <c r="FN14" s="70"/>
+      <c r="FO14" s="70"/>
+      <c r="FP14" s="70"/>
+      <c r="FQ14" s="70"/>
+      <c r="FR14" s="70"/>
+      <c r="FS14" s="70"/>
+      <c r="FT14" s="70"/>
+      <c r="FU14" s="70"/>
+      <c r="FV14" s="70"/>
+      <c r="FW14" s="70"/>
+      <c r="FX14" s="70"/>
+      <c r="FY14" s="70"/>
+      <c r="FZ14" s="70"/>
+      <c r="GA14" s="70"/>
+      <c r="GB14" s="70"/>
+      <c r="GC14" s="70"/>
+      <c r="GD14" s="70"/>
+      <c r="GE14" s="70"/>
+      <c r="GF14" s="70"/>
+      <c r="GG14" s="70"/>
+      <c r="GH14" s="70"/>
+      <c r="GI14" s="70"/>
+      <c r="GJ14" s="70"/>
+      <c r="GK14" s="70"/>
+      <c r="GL14" s="70"/>
+      <c r="GM14" s="70"/>
+      <c r="GN14" s="70"/>
+      <c r="GO14" s="70"/>
+      <c r="GP14" s="70"/>
+      <c r="GQ14" s="70"/>
+      <c r="GR14" s="70"/>
+      <c r="GS14" s="70"/>
+      <c r="GT14" s="70"/>
+      <c r="GU14" s="70"/>
+      <c r="GV14" s="70"/>
+      <c r="GW14" s="70"/>
+      <c r="GX14" s="70"/>
+      <c r="GY14" s="70"/>
+      <c r="GZ14" s="70"/>
+      <c r="HA14" s="70"/>
+      <c r="HB14" s="70"/>
+      <c r="HC14" s="70"/>
+      <c r="HD14" s="70"/>
+      <c r="HE14" s="70"/>
+      <c r="HF14" s="70"/>
+      <c r="HG14" s="70"/>
+      <c r="HH14" s="70"/>
+      <c r="HI14" s="70"/>
+      <c r="HJ14" s="70"/>
+      <c r="HK14" s="70"/>
+      <c r="HL14" s="70"/>
+      <c r="HM14" s="70"/>
+      <c r="HN14" s="70"/>
+      <c r="HO14" s="70"/>
+      <c r="HP14" s="70"/>
+      <c r="HQ14" s="70"/>
+      <c r="HR14" s="70"/>
+      <c r="HS14" s="70"/>
+      <c r="HT14" s="70"/>
+      <c r="HU14" s="70"/>
+      <c r="HV14" s="70"/>
+      <c r="HW14" s="70"/>
+      <c r="HX14" s="70"/>
+      <c r="HY14" s="70"/>
+      <c r="HZ14" s="70"/>
+      <c r="IA14" s="70"/>
+      <c r="IB14" s="70"/>
+      <c r="IC14" s="70"/>
+      <c r="ID14" s="70"/>
+      <c r="IE14" s="70"/>
+      <c r="IF14" s="70"/>
+      <c r="IG14" s="70"/>
+      <c r="IH14" s="70"/>
+      <c r="II14" s="70"/>
+      <c r="IJ14" s="70"/>
+      <c r="IK14" s="70"/>
+      <c r="IL14" s="70"/>
+      <c r="IM14" s="70"/>
+      <c r="IN14" s="70"/>
+      <c r="IO14" s="70"/>
+      <c r="IP14" s="70"/>
+      <c r="IQ14" s="70"/>
+      <c r="IR14" s="70"/>
+      <c r="IS14" s="70"/>
+      <c r="IT14" s="70"/>
+      <c r="IU14" s="70"/>
+      <c r="IV14" s="70"/>
+    </row>
+    <row r="15" spans="1:256" s="71" customFormat="1" ht="111" customHeight="1">
+      <c r="A15" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="27" t="s">
-        <v>45</v>
+      <c r="B15" s="64" t="s">
+        <v>44</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27" t="s">
-        <v>21</v>
+      <c r="C15" s="64" t="s">
+        <v>54</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="31"/>
-      <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="31"/>
-      <c r="AI14" s="31"/>
-      <c r="AJ14" s="31"/>
-      <c r="AK14" s="31"/>
-      <c r="AL14" s="31"/>
-      <c r="AM14" s="31"/>
-      <c r="AN14" s="31"/>
-      <c r="AO14" s="31"/>
-      <c r="AP14" s="31"/>
-      <c r="AQ14" s="31"/>
-      <c r="AR14" s="31"/>
-      <c r="AS14" s="31"/>
-      <c r="AT14" s="31"/>
-      <c r="AU14" s="31"/>
-      <c r="AV14" s="31"/>
-      <c r="AW14" s="31"/>
-      <c r="AX14" s="31"/>
-      <c r="AY14" s="31"/>
-      <c r="AZ14" s="31"/>
-      <c r="BA14" s="31"/>
-      <c r="BB14" s="31"/>
-      <c r="BC14" s="31"/>
-      <c r="BD14" s="31"/>
-      <c r="BE14" s="31"/>
-      <c r="BF14" s="31"/>
-      <c r="BG14" s="31"/>
-      <c r="BH14" s="31"/>
-      <c r="BI14" s="31"/>
-      <c r="BJ14" s="31"/>
-      <c r="BK14" s="31"/>
-      <c r="BL14" s="31"/>
-      <c r="BM14" s="31"/>
-      <c r="BN14" s="31"/>
-      <c r="BO14" s="31"/>
-      <c r="BP14" s="31"/>
-      <c r="BQ14" s="31"/>
-      <c r="BR14" s="31"/>
-      <c r="BS14" s="31"/>
-      <c r="BT14" s="31"/>
-      <c r="BU14" s="31"/>
-      <c r="BV14" s="31"/>
-      <c r="BW14" s="31"/>
-      <c r="BX14" s="31"/>
-      <c r="BY14" s="31"/>
-      <c r="BZ14" s="31"/>
-      <c r="CA14" s="31"/>
-      <c r="CB14" s="31"/>
-      <c r="CC14" s="31"/>
-      <c r="CD14" s="31"/>
-      <c r="CE14" s="31"/>
-      <c r="CF14" s="31"/>
-      <c r="CG14" s="31"/>
-      <c r="CH14" s="31"/>
-      <c r="CI14" s="31"/>
-      <c r="CJ14" s="31"/>
-      <c r="CK14" s="31"/>
-      <c r="CL14" s="31"/>
-      <c r="CM14" s="31"/>
-      <c r="CN14" s="31"/>
-      <c r="CO14" s="31"/>
-      <c r="CP14" s="31"/>
-      <c r="CQ14" s="31"/>
-      <c r="CR14" s="31"/>
-      <c r="CS14" s="31"/>
-      <c r="CT14" s="31"/>
-      <c r="CU14" s="31"/>
-      <c r="CV14" s="31"/>
-      <c r="CW14" s="31"/>
-      <c r="CX14" s="31"/>
-      <c r="CY14" s="31"/>
-      <c r="CZ14" s="31"/>
-      <c r="DA14" s="31"/>
-      <c r="DB14" s="31"/>
-      <c r="DC14" s="31"/>
-      <c r="DD14" s="31"/>
-      <c r="DE14" s="31"/>
-      <c r="DF14" s="31"/>
-      <c r="DG14" s="31"/>
-      <c r="DH14" s="31"/>
-      <c r="DI14" s="31"/>
-      <c r="DJ14" s="31"/>
-      <c r="DK14" s="31"/>
-      <c r="DL14" s="31"/>
-      <c r="DM14" s="31"/>
-      <c r="DN14" s="31"/>
-      <c r="DO14" s="31"/>
-      <c r="DP14" s="31"/>
-      <c r="DQ14" s="31"/>
-      <c r="DR14" s="31"/>
-      <c r="DS14" s="31"/>
-      <c r="DT14" s="31"/>
-      <c r="DU14" s="31"/>
-      <c r="DV14" s="31"/>
-      <c r="DW14" s="31"/>
-      <c r="DX14" s="31"/>
-      <c r="DY14" s="31"/>
-      <c r="DZ14" s="31"/>
-      <c r="EA14" s="31"/>
-      <c r="EB14" s="31"/>
-      <c r="EC14" s="31"/>
-      <c r="ED14" s="31"/>
-      <c r="EE14" s="31"/>
-      <c r="EF14" s="31"/>
-      <c r="EG14" s="31"/>
-      <c r="EH14" s="31"/>
-      <c r="EI14" s="31"/>
-      <c r="EJ14" s="31"/>
-      <c r="EK14" s="31"/>
-      <c r="EL14" s="31"/>
-      <c r="EM14" s="31"/>
-      <c r="EN14" s="31"/>
-      <c r="EO14" s="31"/>
-      <c r="EP14" s="31"/>
-      <c r="EQ14" s="31"/>
-      <c r="ER14" s="31"/>
-      <c r="ES14" s="31"/>
-      <c r="ET14" s="31"/>
-      <c r="EU14" s="31"/>
-      <c r="EV14" s="31"/>
-      <c r="EW14" s="31"/>
-      <c r="EX14" s="31"/>
-      <c r="EY14" s="31"/>
-      <c r="EZ14" s="31"/>
-      <c r="FA14" s="31"/>
-      <c r="FB14" s="31"/>
-      <c r="FC14" s="31"/>
-      <c r="FD14" s="31"/>
-      <c r="FE14" s="31"/>
-      <c r="FF14" s="31"/>
-      <c r="FG14" s="31"/>
-      <c r="FH14" s="31"/>
-      <c r="FI14" s="31"/>
-      <c r="FJ14" s="31"/>
-      <c r="FK14" s="31"/>
-      <c r="FL14" s="31"/>
-      <c r="FM14" s="31"/>
-      <c r="FN14" s="31"/>
-      <c r="FO14" s="31"/>
-      <c r="FP14" s="31"/>
-      <c r="FQ14" s="31"/>
-      <c r="FR14" s="31"/>
-      <c r="FS14" s="31"/>
-      <c r="FT14" s="31"/>
-      <c r="FU14" s="31"/>
-      <c r="FV14" s="31"/>
-      <c r="FW14" s="31"/>
-      <c r="FX14" s="31"/>
-      <c r="FY14" s="31"/>
-      <c r="FZ14" s="31"/>
-      <c r="GA14" s="31"/>
-      <c r="GB14" s="31"/>
-      <c r="GC14" s="31"/>
-      <c r="GD14" s="31"/>
-      <c r="GE14" s="31"/>
-      <c r="GF14" s="31"/>
-      <c r="GG14" s="31"/>
-      <c r="GH14" s="31"/>
-      <c r="GI14" s="31"/>
-      <c r="GJ14" s="31"/>
-      <c r="GK14" s="31"/>
-      <c r="GL14" s="31"/>
-      <c r="GM14" s="31"/>
-      <c r="GN14" s="31"/>
-      <c r="GO14" s="31"/>
-      <c r="GP14" s="31"/>
-      <c r="GQ14" s="31"/>
-      <c r="GR14" s="31"/>
-      <c r="GS14" s="31"/>
-      <c r="GT14" s="31"/>
-      <c r="GU14" s="31"/>
-      <c r="GV14" s="31"/>
-      <c r="GW14" s="31"/>
-      <c r="GX14" s="31"/>
-      <c r="GY14" s="31"/>
-      <c r="GZ14" s="31"/>
-      <c r="HA14" s="31"/>
-      <c r="HB14" s="31"/>
-      <c r="HC14" s="31"/>
-      <c r="HD14" s="31"/>
-      <c r="HE14" s="31"/>
-      <c r="HF14" s="31"/>
-      <c r="HG14" s="31"/>
-      <c r="HH14" s="31"/>
-      <c r="HI14" s="31"/>
-      <c r="HJ14" s="31"/>
-      <c r="HK14" s="31"/>
-      <c r="HL14" s="31"/>
-      <c r="HM14" s="31"/>
-      <c r="HN14" s="31"/>
-      <c r="HO14" s="31"/>
-      <c r="HP14" s="31"/>
-      <c r="HQ14" s="31"/>
-      <c r="HR14" s="31"/>
-      <c r="HS14" s="31"/>
-      <c r="HT14" s="31"/>
-      <c r="HU14" s="31"/>
-      <c r="HV14" s="31"/>
-      <c r="HW14" s="31"/>
-      <c r="HX14" s="31"/>
-      <c r="HY14" s="31"/>
-      <c r="HZ14" s="31"/>
-      <c r="IA14" s="31"/>
-      <c r="IB14" s="31"/>
-      <c r="IC14" s="31"/>
-      <c r="ID14" s="31"/>
-      <c r="IE14" s="31"/>
-      <c r="IF14" s="31"/>
-      <c r="IG14" s="31"/>
-      <c r="IH14" s="31"/>
-      <c r="II14" s="31"/>
-      <c r="IJ14" s="31"/>
-      <c r="IK14" s="31"/>
-      <c r="IL14" s="31"/>
-      <c r="IM14" s="31"/>
-      <c r="IN14" s="31"/>
-      <c r="IO14" s="31"/>
-      <c r="IP14" s="31"/>
-      <c r="IQ14" s="31"/>
-      <c r="IR14" s="31"/>
-      <c r="IS14" s="31"/>
-      <c r="IT14" s="31"/>
-      <c r="IU14" s="31"/>
-      <c r="IV14" s="31"/>
-    </row>
-    <row r="15" spans="1:256" ht="111" customHeight="1">
-      <c r="A15" s="50" t="s">
+      <c r="D15" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="68"/>
+      <c r="Q15" s="68"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="68"/>
+      <c r="V15" s="68"/>
+      <c r="W15" s="68"/>
+      <c r="X15" s="68"/>
+      <c r="Y15" s="68"/>
+      <c r="Z15" s="68"/>
+      <c r="AA15" s="68"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="70"/>
+      <c r="AD15" s="70"/>
+      <c r="AE15" s="70"/>
+      <c r="AF15" s="70"/>
+      <c r="AG15" s="70"/>
+      <c r="AH15" s="70"/>
+      <c r="AI15" s="70"/>
+      <c r="AJ15" s="70"/>
+      <c r="AK15" s="70"/>
+      <c r="AL15" s="70"/>
+      <c r="AM15" s="70"/>
+      <c r="AN15" s="70"/>
+      <c r="AO15" s="70"/>
+      <c r="AP15" s="70"/>
+      <c r="AQ15" s="70"/>
+      <c r="AR15" s="70"/>
+      <c r="AS15" s="70"/>
+      <c r="AT15" s="70"/>
+      <c r="AU15" s="70"/>
+      <c r="AV15" s="70"/>
+      <c r="AW15" s="70"/>
+      <c r="AX15" s="70"/>
+      <c r="AY15" s="70"/>
+      <c r="AZ15" s="70"/>
+      <c r="BA15" s="70"/>
+      <c r="BB15" s="70"/>
+      <c r="BC15" s="70"/>
+      <c r="BD15" s="70"/>
+      <c r="BE15" s="70"/>
+      <c r="BF15" s="70"/>
+      <c r="BG15" s="70"/>
+      <c r="BH15" s="70"/>
+      <c r="BI15" s="70"/>
+      <c r="BJ15" s="70"/>
+      <c r="BK15" s="70"/>
+      <c r="BL15" s="70"/>
+      <c r="BM15" s="70"/>
+      <c r="BN15" s="70"/>
+      <c r="BO15" s="70"/>
+      <c r="BP15" s="70"/>
+      <c r="BQ15" s="70"/>
+      <c r="BR15" s="70"/>
+      <c r="BS15" s="70"/>
+      <c r="BT15" s="70"/>
+      <c r="BU15" s="70"/>
+      <c r="BV15" s="70"/>
+      <c r="BW15" s="70"/>
+      <c r="BX15" s="70"/>
+      <c r="BY15" s="70"/>
+      <c r="BZ15" s="70"/>
+      <c r="CA15" s="70"/>
+      <c r="CB15" s="70"/>
+      <c r="CC15" s="70"/>
+      <c r="CD15" s="70"/>
+      <c r="CE15" s="70"/>
+      <c r="CF15" s="70"/>
+      <c r="CG15" s="70"/>
+      <c r="CH15" s="70"/>
+      <c r="CI15" s="70"/>
+      <c r="CJ15" s="70"/>
+      <c r="CK15" s="70"/>
+      <c r="CL15" s="70"/>
+      <c r="CM15" s="70"/>
+      <c r="CN15" s="70"/>
+      <c r="CO15" s="70"/>
+      <c r="CP15" s="70"/>
+      <c r="CQ15" s="70"/>
+      <c r="CR15" s="70"/>
+      <c r="CS15" s="70"/>
+      <c r="CT15" s="70"/>
+      <c r="CU15" s="70"/>
+      <c r="CV15" s="70"/>
+      <c r="CW15" s="70"/>
+      <c r="CX15" s="70"/>
+      <c r="CY15" s="70"/>
+      <c r="CZ15" s="70"/>
+      <c r="DA15" s="70"/>
+      <c r="DB15" s="70"/>
+      <c r="DC15" s="70"/>
+      <c r="DD15" s="70"/>
+      <c r="DE15" s="70"/>
+      <c r="DF15" s="70"/>
+      <c r="DG15" s="70"/>
+      <c r="DH15" s="70"/>
+      <c r="DI15" s="70"/>
+      <c r="DJ15" s="70"/>
+      <c r="DK15" s="70"/>
+      <c r="DL15" s="70"/>
+      <c r="DM15" s="70"/>
+      <c r="DN15" s="70"/>
+      <c r="DO15" s="70"/>
+      <c r="DP15" s="70"/>
+      <c r="DQ15" s="70"/>
+      <c r="DR15" s="70"/>
+      <c r="DS15" s="70"/>
+      <c r="DT15" s="70"/>
+      <c r="DU15" s="70"/>
+      <c r="DV15" s="70"/>
+      <c r="DW15" s="70"/>
+      <c r="DX15" s="70"/>
+      <c r="DY15" s="70"/>
+      <c r="DZ15" s="70"/>
+      <c r="EA15" s="70"/>
+      <c r="EB15" s="70"/>
+      <c r="EC15" s="70"/>
+      <c r="ED15" s="70"/>
+      <c r="EE15" s="70"/>
+      <c r="EF15" s="70"/>
+      <c r="EG15" s="70"/>
+      <c r="EH15" s="70"/>
+      <c r="EI15" s="70"/>
+      <c r="EJ15" s="70"/>
+      <c r="EK15" s="70"/>
+      <c r="EL15" s="70"/>
+      <c r="EM15" s="70"/>
+      <c r="EN15" s="70"/>
+      <c r="EO15" s="70"/>
+      <c r="EP15" s="70"/>
+      <c r="EQ15" s="70"/>
+      <c r="ER15" s="70"/>
+      <c r="ES15" s="70"/>
+      <c r="ET15" s="70"/>
+      <c r="EU15" s="70"/>
+      <c r="EV15" s="70"/>
+      <c r="EW15" s="70"/>
+      <c r="EX15" s="70"/>
+      <c r="EY15" s="70"/>
+      <c r="EZ15" s="70"/>
+      <c r="FA15" s="70"/>
+      <c r="FB15" s="70"/>
+      <c r="FC15" s="70"/>
+      <c r="FD15" s="70"/>
+      <c r="FE15" s="70"/>
+      <c r="FF15" s="70"/>
+      <c r="FG15" s="70"/>
+      <c r="FH15" s="70"/>
+      <c r="FI15" s="70"/>
+      <c r="FJ15" s="70"/>
+      <c r="FK15" s="70"/>
+      <c r="FL15" s="70"/>
+      <c r="FM15" s="70"/>
+      <c r="FN15" s="70"/>
+      <c r="FO15" s="70"/>
+      <c r="FP15" s="70"/>
+      <c r="FQ15" s="70"/>
+      <c r="FR15" s="70"/>
+      <c r="FS15" s="70"/>
+      <c r="FT15" s="70"/>
+      <c r="FU15" s="70"/>
+      <c r="FV15" s="70"/>
+      <c r="FW15" s="70"/>
+      <c r="FX15" s="70"/>
+      <c r="FY15" s="70"/>
+      <c r="FZ15" s="70"/>
+      <c r="GA15" s="70"/>
+      <c r="GB15" s="70"/>
+      <c r="GC15" s="70"/>
+      <c r="GD15" s="70"/>
+      <c r="GE15" s="70"/>
+      <c r="GF15" s="70"/>
+      <c r="GG15" s="70"/>
+      <c r="GH15" s="70"/>
+      <c r="GI15" s="70"/>
+      <c r="GJ15" s="70"/>
+      <c r="GK15" s="70"/>
+      <c r="GL15" s="70"/>
+      <c r="GM15" s="70"/>
+      <c r="GN15" s="70"/>
+      <c r="GO15" s="70"/>
+      <c r="GP15" s="70"/>
+      <c r="GQ15" s="70"/>
+      <c r="GR15" s="70"/>
+      <c r="GS15" s="70"/>
+      <c r="GT15" s="70"/>
+      <c r="GU15" s="70"/>
+      <c r="GV15" s="70"/>
+      <c r="GW15" s="70"/>
+      <c r="GX15" s="70"/>
+      <c r="GY15" s="70"/>
+      <c r="GZ15" s="70"/>
+      <c r="HA15" s="70"/>
+      <c r="HB15" s="70"/>
+      <c r="HC15" s="70"/>
+      <c r="HD15" s="70"/>
+      <c r="HE15" s="70"/>
+      <c r="HF15" s="70"/>
+      <c r="HG15" s="70"/>
+      <c r="HH15" s="70"/>
+      <c r="HI15" s="70"/>
+      <c r="HJ15" s="70"/>
+      <c r="HK15" s="70"/>
+      <c r="HL15" s="70"/>
+      <c r="HM15" s="70"/>
+      <c r="HN15" s="70"/>
+      <c r="HO15" s="70"/>
+      <c r="HP15" s="70"/>
+      <c r="HQ15" s="70"/>
+      <c r="HR15" s="70"/>
+      <c r="HS15" s="70"/>
+      <c r="HT15" s="70"/>
+      <c r="HU15" s="70"/>
+      <c r="HV15" s="70"/>
+      <c r="HW15" s="70"/>
+      <c r="HX15" s="70"/>
+      <c r="HY15" s="70"/>
+      <c r="HZ15" s="70"/>
+      <c r="IA15" s="70"/>
+      <c r="IB15" s="70"/>
+      <c r="IC15" s="70"/>
+      <c r="ID15" s="70"/>
+      <c r="IE15" s="70"/>
+      <c r="IF15" s="70"/>
+      <c r="IG15" s="70"/>
+      <c r="IH15" s="70"/>
+      <c r="II15" s="70"/>
+      <c r="IJ15" s="70"/>
+      <c r="IK15" s="70"/>
+      <c r="IL15" s="70"/>
+      <c r="IM15" s="70"/>
+      <c r="IN15" s="70"/>
+      <c r="IO15" s="70"/>
+      <c r="IP15" s="70"/>
+      <c r="IQ15" s="70"/>
+      <c r="IR15" s="70"/>
+      <c r="IS15" s="70"/>
+      <c r="IT15" s="70"/>
+      <c r="IU15" s="70"/>
+      <c r="IV15" s="70"/>
+    </row>
+    <row r="16" spans="1:256" s="71" customFormat="1" ht="99.6" customHeight="1">
+      <c r="A16" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>45</v>
+      <c r="B16" s="64" t="s">
+        <v>44</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27" t="s">
-        <v>21</v>
+      <c r="C16" s="64" t="s">
+        <v>55</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="32"/>
-      <c r="AA15" s="32"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="31"/>
-      <c r="AD15" s="31"/>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31"/>
-      <c r="AG15" s="31"/>
-      <c r="AH15" s="31"/>
-      <c r="AI15" s="31"/>
-      <c r="AJ15" s="31"/>
-      <c r="AK15" s="31"/>
-      <c r="AL15" s="31"/>
-      <c r="AM15" s="31"/>
-      <c r="AN15" s="31"/>
-      <c r="AO15" s="31"/>
-      <c r="AP15" s="31"/>
-      <c r="AQ15" s="31"/>
-      <c r="AR15" s="31"/>
-      <c r="AS15" s="31"/>
-      <c r="AT15" s="31"/>
-      <c r="AU15" s="31"/>
-      <c r="AV15" s="31"/>
-      <c r="AW15" s="31"/>
-      <c r="AX15" s="31"/>
-      <c r="AY15" s="31"/>
-      <c r="AZ15" s="31"/>
-      <c r="BA15" s="31"/>
-      <c r="BB15" s="31"/>
-      <c r="BC15" s="31"/>
-      <c r="BD15" s="31"/>
-      <c r="BE15" s="31"/>
-      <c r="BF15" s="31"/>
-      <c r="BG15" s="31"/>
-      <c r="BH15" s="31"/>
-      <c r="BI15" s="31"/>
-      <c r="BJ15" s="31"/>
-      <c r="BK15" s="31"/>
-      <c r="BL15" s="31"/>
-      <c r="BM15" s="31"/>
-      <c r="BN15" s="31"/>
-      <c r="BO15" s="31"/>
-      <c r="BP15" s="31"/>
-      <c r="BQ15" s="31"/>
-      <c r="BR15" s="31"/>
-      <c r="BS15" s="31"/>
-      <c r="BT15" s="31"/>
-      <c r="BU15" s="31"/>
-      <c r="BV15" s="31"/>
-      <c r="BW15" s="31"/>
-      <c r="BX15" s="31"/>
-      <c r="BY15" s="31"/>
-      <c r="BZ15" s="31"/>
-      <c r="CA15" s="31"/>
-      <c r="CB15" s="31"/>
-      <c r="CC15" s="31"/>
-      <c r="CD15" s="31"/>
-      <c r="CE15" s="31"/>
-      <c r="CF15" s="31"/>
-      <c r="CG15" s="31"/>
-      <c r="CH15" s="31"/>
-      <c r="CI15" s="31"/>
-      <c r="CJ15" s="31"/>
-      <c r="CK15" s="31"/>
-      <c r="CL15" s="31"/>
-      <c r="CM15" s="31"/>
-      <c r="CN15" s="31"/>
-      <c r="CO15" s="31"/>
-      <c r="CP15" s="31"/>
-      <c r="CQ15" s="31"/>
-      <c r="CR15" s="31"/>
-      <c r="CS15" s="31"/>
-      <c r="CT15" s="31"/>
-      <c r="CU15" s="31"/>
-      <c r="CV15" s="31"/>
-      <c r="CW15" s="31"/>
-      <c r="CX15" s="31"/>
-      <c r="CY15" s="31"/>
-      <c r="CZ15" s="31"/>
-      <c r="DA15" s="31"/>
-      <c r="DB15" s="31"/>
-      <c r="DC15" s="31"/>
-      <c r="DD15" s="31"/>
-      <c r="DE15" s="31"/>
-      <c r="DF15" s="31"/>
-      <c r="DG15" s="31"/>
-      <c r="DH15" s="31"/>
-      <c r="DI15" s="31"/>
-      <c r="DJ15" s="31"/>
-      <c r="DK15" s="31"/>
-      <c r="DL15" s="31"/>
-      <c r="DM15" s="31"/>
-      <c r="DN15" s="31"/>
-      <c r="DO15" s="31"/>
-      <c r="DP15" s="31"/>
-      <c r="DQ15" s="31"/>
-      <c r="DR15" s="31"/>
-      <c r="DS15" s="31"/>
-      <c r="DT15" s="31"/>
-      <c r="DU15" s="31"/>
-      <c r="DV15" s="31"/>
-      <c r="DW15" s="31"/>
-      <c r="DX15" s="31"/>
-      <c r="DY15" s="31"/>
-      <c r="DZ15" s="31"/>
-      <c r="EA15" s="31"/>
-      <c r="EB15" s="31"/>
-      <c r="EC15" s="31"/>
-      <c r="ED15" s="31"/>
-      <c r="EE15" s="31"/>
-      <c r="EF15" s="31"/>
-      <c r="EG15" s="31"/>
-      <c r="EH15" s="31"/>
-      <c r="EI15" s="31"/>
-      <c r="EJ15" s="31"/>
-      <c r="EK15" s="31"/>
-      <c r="EL15" s="31"/>
-      <c r="EM15" s="31"/>
-      <c r="EN15" s="31"/>
-      <c r="EO15" s="31"/>
-      <c r="EP15" s="31"/>
-      <c r="EQ15" s="31"/>
-      <c r="ER15" s="31"/>
-      <c r="ES15" s="31"/>
-      <c r="ET15" s="31"/>
-      <c r="EU15" s="31"/>
-      <c r="EV15" s="31"/>
-      <c r="EW15" s="31"/>
-      <c r="EX15" s="31"/>
-      <c r="EY15" s="31"/>
-      <c r="EZ15" s="31"/>
-      <c r="FA15" s="31"/>
-      <c r="FB15" s="31"/>
-      <c r="FC15" s="31"/>
-      <c r="FD15" s="31"/>
-      <c r="FE15" s="31"/>
-      <c r="FF15" s="31"/>
-      <c r="FG15" s="31"/>
-      <c r="FH15" s="31"/>
-      <c r="FI15" s="31"/>
-      <c r="FJ15" s="31"/>
-      <c r="FK15" s="31"/>
-      <c r="FL15" s="31"/>
-      <c r="FM15" s="31"/>
-      <c r="FN15" s="31"/>
-      <c r="FO15" s="31"/>
-      <c r="FP15" s="31"/>
-      <c r="FQ15" s="31"/>
-      <c r="FR15" s="31"/>
-      <c r="FS15" s="31"/>
-      <c r="FT15" s="31"/>
-      <c r="FU15" s="31"/>
-      <c r="FV15" s="31"/>
-      <c r="FW15" s="31"/>
-      <c r="FX15" s="31"/>
-      <c r="FY15" s="31"/>
-      <c r="FZ15" s="31"/>
-      <c r="GA15" s="31"/>
-      <c r="GB15" s="31"/>
-      <c r="GC15" s="31"/>
-      <c r="GD15" s="31"/>
-      <c r="GE15" s="31"/>
-      <c r="GF15" s="31"/>
-      <c r="GG15" s="31"/>
-      <c r="GH15" s="31"/>
-      <c r="GI15" s="31"/>
-      <c r="GJ15" s="31"/>
-      <c r="GK15" s="31"/>
-      <c r="GL15" s="31"/>
-      <c r="GM15" s="31"/>
-      <c r="GN15" s="31"/>
-      <c r="GO15" s="31"/>
-      <c r="GP15" s="31"/>
-      <c r="GQ15" s="31"/>
-      <c r="GR15" s="31"/>
-      <c r="GS15" s="31"/>
-      <c r="GT15" s="31"/>
-      <c r="GU15" s="31"/>
-      <c r="GV15" s="31"/>
-      <c r="GW15" s="31"/>
-      <c r="GX15" s="31"/>
-      <c r="GY15" s="31"/>
-      <c r="GZ15" s="31"/>
-      <c r="HA15" s="31"/>
-      <c r="HB15" s="31"/>
-      <c r="HC15" s="31"/>
-      <c r="HD15" s="31"/>
-      <c r="HE15" s="31"/>
-      <c r="HF15" s="31"/>
-      <c r="HG15" s="31"/>
-      <c r="HH15" s="31"/>
-      <c r="HI15" s="31"/>
-      <c r="HJ15" s="31"/>
-      <c r="HK15" s="31"/>
-      <c r="HL15" s="31"/>
-      <c r="HM15" s="31"/>
-      <c r="HN15" s="31"/>
-      <c r="HO15" s="31"/>
-      <c r="HP15" s="31"/>
-      <c r="HQ15" s="31"/>
-      <c r="HR15" s="31"/>
-      <c r="HS15" s="31"/>
-      <c r="HT15" s="31"/>
-      <c r="HU15" s="31"/>
-      <c r="HV15" s="31"/>
-      <c r="HW15" s="31"/>
-      <c r="HX15" s="31"/>
-      <c r="HY15" s="31"/>
-      <c r="HZ15" s="31"/>
-      <c r="IA15" s="31"/>
-      <c r="IB15" s="31"/>
-      <c r="IC15" s="31"/>
-      <c r="ID15" s="31"/>
-      <c r="IE15" s="31"/>
-      <c r="IF15" s="31"/>
-      <c r="IG15" s="31"/>
-      <c r="IH15" s="31"/>
-      <c r="II15" s="31"/>
-      <c r="IJ15" s="31"/>
-      <c r="IK15" s="31"/>
-      <c r="IL15" s="31"/>
-      <c r="IM15" s="31"/>
-      <c r="IN15" s="31"/>
-      <c r="IO15" s="31"/>
-      <c r="IP15" s="31"/>
-      <c r="IQ15" s="31"/>
-      <c r="IR15" s="31"/>
-      <c r="IS15" s="31"/>
-      <c r="IT15" s="31"/>
-      <c r="IU15" s="31"/>
-      <c r="IV15" s="31"/>
-    </row>
-    <row r="16" spans="1:256" ht="99.6" customHeight="1">
-      <c r="A16" s="50" t="s">
+      <c r="D16" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="68"/>
+      <c r="R16" s="68"/>
+      <c r="S16" s="68"/>
+      <c r="T16" s="68"/>
+      <c r="U16" s="68"/>
+      <c r="V16" s="68"/>
+      <c r="W16" s="68"/>
+      <c r="X16" s="68"/>
+      <c r="Y16" s="68"/>
+      <c r="Z16" s="68"/>
+      <c r="AA16" s="68"/>
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="70"/>
+      <c r="AD16" s="70"/>
+      <c r="AE16" s="70"/>
+      <c r="AF16" s="70"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
+      <c r="AL16" s="70"/>
+      <c r="AM16" s="70"/>
+      <c r="AN16" s="70"/>
+      <c r="AO16" s="70"/>
+      <c r="AP16" s="70"/>
+      <c r="AQ16" s="70"/>
+      <c r="AR16" s="70"/>
+      <c r="AS16" s="70"/>
+      <c r="AT16" s="70"/>
+      <c r="AU16" s="70"/>
+      <c r="AV16" s="70"/>
+      <c r="AW16" s="70"/>
+      <c r="AX16" s="70"/>
+      <c r="AY16" s="70"/>
+      <c r="AZ16" s="70"/>
+      <c r="BA16" s="70"/>
+      <c r="BB16" s="70"/>
+      <c r="BC16" s="70"/>
+      <c r="BD16" s="70"/>
+      <c r="BE16" s="70"/>
+      <c r="BF16" s="70"/>
+      <c r="BG16" s="70"/>
+      <c r="BH16" s="70"/>
+      <c r="BI16" s="70"/>
+      <c r="BJ16" s="70"/>
+      <c r="BK16" s="70"/>
+      <c r="BL16" s="70"/>
+      <c r="BM16" s="70"/>
+      <c r="BN16" s="70"/>
+      <c r="BO16" s="70"/>
+      <c r="BP16" s="70"/>
+      <c r="BQ16" s="70"/>
+      <c r="BR16" s="70"/>
+      <c r="BS16" s="70"/>
+      <c r="BT16" s="70"/>
+      <c r="BU16" s="70"/>
+      <c r="BV16" s="70"/>
+      <c r="BW16" s="70"/>
+      <c r="BX16" s="70"/>
+      <c r="BY16" s="70"/>
+      <c r="BZ16" s="70"/>
+      <c r="CA16" s="70"/>
+      <c r="CB16" s="70"/>
+      <c r="CC16" s="70"/>
+      <c r="CD16" s="70"/>
+      <c r="CE16" s="70"/>
+      <c r="CF16" s="70"/>
+      <c r="CG16" s="70"/>
+      <c r="CH16" s="70"/>
+      <c r="CI16" s="70"/>
+      <c r="CJ16" s="70"/>
+      <c r="CK16" s="70"/>
+      <c r="CL16" s="70"/>
+      <c r="CM16" s="70"/>
+      <c r="CN16" s="70"/>
+      <c r="CO16" s="70"/>
+      <c r="CP16" s="70"/>
+      <c r="CQ16" s="70"/>
+      <c r="CR16" s="70"/>
+      <c r="CS16" s="70"/>
+      <c r="CT16" s="70"/>
+      <c r="CU16" s="70"/>
+      <c r="CV16" s="70"/>
+      <c r="CW16" s="70"/>
+      <c r="CX16" s="70"/>
+      <c r="CY16" s="70"/>
+      <c r="CZ16" s="70"/>
+      <c r="DA16" s="70"/>
+      <c r="DB16" s="70"/>
+      <c r="DC16" s="70"/>
+      <c r="DD16" s="70"/>
+      <c r="DE16" s="70"/>
+      <c r="DF16" s="70"/>
+      <c r="DG16" s="70"/>
+      <c r="DH16" s="70"/>
+      <c r="DI16" s="70"/>
+      <c r="DJ16" s="70"/>
+      <c r="DK16" s="70"/>
+      <c r="DL16" s="70"/>
+      <c r="DM16" s="70"/>
+      <c r="DN16" s="70"/>
+      <c r="DO16" s="70"/>
+      <c r="DP16" s="70"/>
+      <c r="DQ16" s="70"/>
+      <c r="DR16" s="70"/>
+      <c r="DS16" s="70"/>
+      <c r="DT16" s="70"/>
+      <c r="DU16" s="70"/>
+      <c r="DV16" s="70"/>
+      <c r="DW16" s="70"/>
+      <c r="DX16" s="70"/>
+      <c r="DY16" s="70"/>
+      <c r="DZ16" s="70"/>
+      <c r="EA16" s="70"/>
+      <c r="EB16" s="70"/>
+      <c r="EC16" s="70"/>
+      <c r="ED16" s="70"/>
+      <c r="EE16" s="70"/>
+      <c r="EF16" s="70"/>
+      <c r="EG16" s="70"/>
+      <c r="EH16" s="70"/>
+      <c r="EI16" s="70"/>
+      <c r="EJ16" s="70"/>
+      <c r="EK16" s="70"/>
+      <c r="EL16" s="70"/>
+      <c r="EM16" s="70"/>
+      <c r="EN16" s="70"/>
+      <c r="EO16" s="70"/>
+      <c r="EP16" s="70"/>
+      <c r="EQ16" s="70"/>
+      <c r="ER16" s="70"/>
+      <c r="ES16" s="70"/>
+      <c r="ET16" s="70"/>
+      <c r="EU16" s="70"/>
+      <c r="EV16" s="70"/>
+      <c r="EW16" s="70"/>
+      <c r="EX16" s="70"/>
+      <c r="EY16" s="70"/>
+      <c r="EZ16" s="70"/>
+      <c r="FA16" s="70"/>
+      <c r="FB16" s="70"/>
+      <c r="FC16" s="70"/>
+      <c r="FD16" s="70"/>
+      <c r="FE16" s="70"/>
+      <c r="FF16" s="70"/>
+      <c r="FG16" s="70"/>
+      <c r="FH16" s="70"/>
+      <c r="FI16" s="70"/>
+      <c r="FJ16" s="70"/>
+      <c r="FK16" s="70"/>
+      <c r="FL16" s="70"/>
+      <c r="FM16" s="70"/>
+      <c r="FN16" s="70"/>
+      <c r="FO16" s="70"/>
+      <c r="FP16" s="70"/>
+      <c r="FQ16" s="70"/>
+      <c r="FR16" s="70"/>
+      <c r="FS16" s="70"/>
+      <c r="FT16" s="70"/>
+      <c r="FU16" s="70"/>
+      <c r="FV16" s="70"/>
+      <c r="FW16" s="70"/>
+      <c r="FX16" s="70"/>
+      <c r="FY16" s="70"/>
+      <c r="FZ16" s="70"/>
+      <c r="GA16" s="70"/>
+      <c r="GB16" s="70"/>
+      <c r="GC16" s="70"/>
+      <c r="GD16" s="70"/>
+      <c r="GE16" s="70"/>
+      <c r="GF16" s="70"/>
+      <c r="GG16" s="70"/>
+      <c r="GH16" s="70"/>
+      <c r="GI16" s="70"/>
+      <c r="GJ16" s="70"/>
+      <c r="GK16" s="70"/>
+      <c r="GL16" s="70"/>
+      <c r="GM16" s="70"/>
+      <c r="GN16" s="70"/>
+      <c r="GO16" s="70"/>
+      <c r="GP16" s="70"/>
+      <c r="GQ16" s="70"/>
+      <c r="GR16" s="70"/>
+      <c r="GS16" s="70"/>
+      <c r="GT16" s="70"/>
+      <c r="GU16" s="70"/>
+      <c r="GV16" s="70"/>
+      <c r="GW16" s="70"/>
+      <c r="GX16" s="70"/>
+      <c r="GY16" s="70"/>
+      <c r="GZ16" s="70"/>
+      <c r="HA16" s="70"/>
+      <c r="HB16" s="70"/>
+      <c r="HC16" s="70"/>
+      <c r="HD16" s="70"/>
+      <c r="HE16" s="70"/>
+      <c r="HF16" s="70"/>
+      <c r="HG16" s="70"/>
+      <c r="HH16" s="70"/>
+      <c r="HI16" s="70"/>
+      <c r="HJ16" s="70"/>
+      <c r="HK16" s="70"/>
+      <c r="HL16" s="70"/>
+      <c r="HM16" s="70"/>
+      <c r="HN16" s="70"/>
+      <c r="HO16" s="70"/>
+      <c r="HP16" s="70"/>
+      <c r="HQ16" s="70"/>
+      <c r="HR16" s="70"/>
+      <c r="HS16" s="70"/>
+      <c r="HT16" s="70"/>
+      <c r="HU16" s="70"/>
+      <c r="HV16" s="70"/>
+      <c r="HW16" s="70"/>
+      <c r="HX16" s="70"/>
+      <c r="HY16" s="70"/>
+      <c r="HZ16" s="70"/>
+      <c r="IA16" s="70"/>
+      <c r="IB16" s="70"/>
+      <c r="IC16" s="70"/>
+      <c r="ID16" s="70"/>
+      <c r="IE16" s="70"/>
+      <c r="IF16" s="70"/>
+      <c r="IG16" s="70"/>
+      <c r="IH16" s="70"/>
+      <c r="II16" s="70"/>
+      <c r="IJ16" s="70"/>
+      <c r="IK16" s="70"/>
+      <c r="IL16" s="70"/>
+      <c r="IM16" s="70"/>
+      <c r="IN16" s="70"/>
+      <c r="IO16" s="70"/>
+      <c r="IP16" s="70"/>
+      <c r="IQ16" s="70"/>
+      <c r="IR16" s="70"/>
+      <c r="IS16" s="70"/>
+      <c r="IT16" s="70"/>
+      <c r="IU16" s="70"/>
+      <c r="IV16" s="70"/>
+    </row>
+    <row r="17" spans="1:256" s="62" customFormat="1" ht="348" hidden="1" customHeight="1">
+      <c r="A17" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>45</v>
+      <c r="B17" s="55" t="s">
+        <v>43</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27" t="s">
-        <v>21</v>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55" t="s">
+        <v>20</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="32"/>
-      <c r="X16" s="32"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="31"/>
-      <c r="AD16" s="31"/>
-      <c r="AE16" s="31"/>
-      <c r="AF16" s="31"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="31"/>
-      <c r="AI16" s="31"/>
-      <c r="AJ16" s="31"/>
-      <c r="AK16" s="31"/>
-      <c r="AL16" s="31"/>
-      <c r="AM16" s="31"/>
-      <c r="AN16" s="31"/>
-      <c r="AO16" s="31"/>
-      <c r="AP16" s="31"/>
-      <c r="AQ16" s="31"/>
-      <c r="AR16" s="31"/>
-      <c r="AS16" s="31"/>
-      <c r="AT16" s="31"/>
-      <c r="AU16" s="31"/>
-      <c r="AV16" s="31"/>
-      <c r="AW16" s="31"/>
-      <c r="AX16" s="31"/>
-      <c r="AY16" s="31"/>
-      <c r="AZ16" s="31"/>
-      <c r="BA16" s="31"/>
-      <c r="BB16" s="31"/>
-      <c r="BC16" s="31"/>
-      <c r="BD16" s="31"/>
-      <c r="BE16" s="31"/>
-      <c r="BF16" s="31"/>
-      <c r="BG16" s="31"/>
-      <c r="BH16" s="31"/>
-      <c r="BI16" s="31"/>
-      <c r="BJ16" s="31"/>
-      <c r="BK16" s="31"/>
-      <c r="BL16" s="31"/>
-      <c r="BM16" s="31"/>
-      <c r="BN16" s="31"/>
-      <c r="BO16" s="31"/>
-      <c r="BP16" s="31"/>
-      <c r="BQ16" s="31"/>
-      <c r="BR16" s="31"/>
-      <c r="BS16" s="31"/>
-      <c r="BT16" s="31"/>
-      <c r="BU16" s="31"/>
-      <c r="BV16" s="31"/>
-      <c r="BW16" s="31"/>
-      <c r="BX16" s="31"/>
-      <c r="BY16" s="31"/>
-      <c r="BZ16" s="31"/>
-      <c r="CA16" s="31"/>
-      <c r="CB16" s="31"/>
-      <c r="CC16" s="31"/>
-      <c r="CD16" s="31"/>
-      <c r="CE16" s="31"/>
-      <c r="CF16" s="31"/>
-      <c r="CG16" s="31"/>
-      <c r="CH16" s="31"/>
-      <c r="CI16" s="31"/>
-      <c r="CJ16" s="31"/>
-      <c r="CK16" s="31"/>
-      <c r="CL16" s="31"/>
-      <c r="CM16" s="31"/>
-      <c r="CN16" s="31"/>
-      <c r="CO16" s="31"/>
-      <c r="CP16" s="31"/>
-      <c r="CQ16" s="31"/>
-      <c r="CR16" s="31"/>
-      <c r="CS16" s="31"/>
-      <c r="CT16" s="31"/>
-      <c r="CU16" s="31"/>
-      <c r="CV16" s="31"/>
-      <c r="CW16" s="31"/>
-      <c r="CX16" s="31"/>
-      <c r="CY16" s="31"/>
-      <c r="CZ16" s="31"/>
-      <c r="DA16" s="31"/>
-      <c r="DB16" s="31"/>
-      <c r="DC16" s="31"/>
-      <c r="DD16" s="31"/>
-      <c r="DE16" s="31"/>
-      <c r="DF16" s="31"/>
-      <c r="DG16" s="31"/>
-      <c r="DH16" s="31"/>
-      <c r="DI16" s="31"/>
-      <c r="DJ16" s="31"/>
-      <c r="DK16" s="31"/>
-      <c r="DL16" s="31"/>
-      <c r="DM16" s="31"/>
-      <c r="DN16" s="31"/>
-      <c r="DO16" s="31"/>
-      <c r="DP16" s="31"/>
-      <c r="DQ16" s="31"/>
-      <c r="DR16" s="31"/>
-      <c r="DS16" s="31"/>
-      <c r="DT16" s="31"/>
-      <c r="DU16" s="31"/>
-      <c r="DV16" s="31"/>
-      <c r="DW16" s="31"/>
-      <c r="DX16" s="31"/>
-      <c r="DY16" s="31"/>
-      <c r="DZ16" s="31"/>
-      <c r="EA16" s="31"/>
-      <c r="EB16" s="31"/>
-      <c r="EC16" s="31"/>
-      <c r="ED16" s="31"/>
-      <c r="EE16" s="31"/>
-      <c r="EF16" s="31"/>
-      <c r="EG16" s="31"/>
-      <c r="EH16" s="31"/>
-      <c r="EI16" s="31"/>
-      <c r="EJ16" s="31"/>
-      <c r="EK16" s="31"/>
-      <c r="EL16" s="31"/>
-      <c r="EM16" s="31"/>
-      <c r="EN16" s="31"/>
-      <c r="EO16" s="31"/>
-      <c r="EP16" s="31"/>
-      <c r="EQ16" s="31"/>
-      <c r="ER16" s="31"/>
-      <c r="ES16" s="31"/>
-      <c r="ET16" s="31"/>
-      <c r="EU16" s="31"/>
-      <c r="EV16" s="31"/>
-      <c r="EW16" s="31"/>
-      <c r="EX16" s="31"/>
-      <c r="EY16" s="31"/>
-      <c r="EZ16" s="31"/>
-      <c r="FA16" s="31"/>
-      <c r="FB16" s="31"/>
-      <c r="FC16" s="31"/>
-      <c r="FD16" s="31"/>
-      <c r="FE16" s="31"/>
-      <c r="FF16" s="31"/>
-      <c r="FG16" s="31"/>
-      <c r="FH16" s="31"/>
-      <c r="FI16" s="31"/>
-      <c r="FJ16" s="31"/>
-      <c r="FK16" s="31"/>
-      <c r="FL16" s="31"/>
-      <c r="FM16" s="31"/>
-      <c r="FN16" s="31"/>
-      <c r="FO16" s="31"/>
-      <c r="FP16" s="31"/>
-      <c r="FQ16" s="31"/>
-      <c r="FR16" s="31"/>
-      <c r="FS16" s="31"/>
-      <c r="FT16" s="31"/>
-      <c r="FU16" s="31"/>
-      <c r="FV16" s="31"/>
-      <c r="FW16" s="31"/>
-      <c r="FX16" s="31"/>
-      <c r="FY16" s="31"/>
-      <c r="FZ16" s="31"/>
-      <c r="GA16" s="31"/>
-      <c r="GB16" s="31"/>
-      <c r="GC16" s="31"/>
-      <c r="GD16" s="31"/>
-      <c r="GE16" s="31"/>
-      <c r="GF16" s="31"/>
-      <c r="GG16" s="31"/>
-      <c r="GH16" s="31"/>
-      <c r="GI16" s="31"/>
-      <c r="GJ16" s="31"/>
-      <c r="GK16" s="31"/>
-      <c r="GL16" s="31"/>
-      <c r="GM16" s="31"/>
-      <c r="GN16" s="31"/>
-      <c r="GO16" s="31"/>
-      <c r="GP16" s="31"/>
-      <c r="GQ16" s="31"/>
-      <c r="GR16" s="31"/>
-      <c r="GS16" s="31"/>
-      <c r="GT16" s="31"/>
-      <c r="GU16" s="31"/>
-      <c r="GV16" s="31"/>
-      <c r="GW16" s="31"/>
-      <c r="GX16" s="31"/>
-      <c r="GY16" s="31"/>
-      <c r="GZ16" s="31"/>
-      <c r="HA16" s="31"/>
-      <c r="HB16" s="31"/>
-      <c r="HC16" s="31"/>
-      <c r="HD16" s="31"/>
-      <c r="HE16" s="31"/>
-      <c r="HF16" s="31"/>
-      <c r="HG16" s="31"/>
-      <c r="HH16" s="31"/>
-      <c r="HI16" s="31"/>
-      <c r="HJ16" s="31"/>
-      <c r="HK16" s="31"/>
-      <c r="HL16" s="31"/>
-      <c r="HM16" s="31"/>
-      <c r="HN16" s="31"/>
-      <c r="HO16" s="31"/>
-      <c r="HP16" s="31"/>
-      <c r="HQ16" s="31"/>
-      <c r="HR16" s="31"/>
-      <c r="HS16" s="31"/>
-      <c r="HT16" s="31"/>
-      <c r="HU16" s="31"/>
-      <c r="HV16" s="31"/>
-      <c r="HW16" s="31"/>
-      <c r="HX16" s="31"/>
-      <c r="HY16" s="31"/>
-      <c r="HZ16" s="31"/>
-      <c r="IA16" s="31"/>
-      <c r="IB16" s="31"/>
-      <c r="IC16" s="31"/>
-      <c r="ID16" s="31"/>
-      <c r="IE16" s="31"/>
-      <c r="IF16" s="31"/>
-      <c r="IG16" s="31"/>
-      <c r="IH16" s="31"/>
-      <c r="II16" s="31"/>
-      <c r="IJ16" s="31"/>
-      <c r="IK16" s="31"/>
-      <c r="IL16" s="31"/>
-      <c r="IM16" s="31"/>
-      <c r="IN16" s="31"/>
-      <c r="IO16" s="31"/>
-      <c r="IP16" s="31"/>
-      <c r="IQ16" s="31"/>
-      <c r="IR16" s="31"/>
-      <c r="IS16" s="31"/>
-      <c r="IT16" s="31"/>
-      <c r="IU16" s="31"/>
-      <c r="IV16" s="31"/>
-    </row>
-    <row r="17" spans="1:256" ht="348" customHeight="1">
-      <c r="A17" s="50" t="s">
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="59"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
+      <c r="Y17" s="59"/>
+      <c r="Z17" s="59"/>
+      <c r="AA17" s="59"/>
+      <c r="AB17" s="60"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
+      <c r="AG17" s="61"/>
+      <c r="AH17" s="61"/>
+      <c r="AI17" s="61"/>
+      <c r="AJ17" s="61"/>
+      <c r="AK17" s="61"/>
+      <c r="AL17" s="61"/>
+      <c r="AM17" s="61"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="61"/>
+      <c r="AP17" s="61"/>
+      <c r="AQ17" s="61"/>
+      <c r="AR17" s="61"/>
+      <c r="AS17" s="61"/>
+      <c r="AT17" s="61"/>
+      <c r="AU17" s="61"/>
+      <c r="AV17" s="61"/>
+      <c r="AW17" s="61"/>
+      <c r="AX17" s="61"/>
+      <c r="AY17" s="61"/>
+      <c r="AZ17" s="61"/>
+      <c r="BA17" s="61"/>
+      <c r="BB17" s="61"/>
+      <c r="BC17" s="61"/>
+      <c r="BD17" s="61"/>
+      <c r="BE17" s="61"/>
+      <c r="BF17" s="61"/>
+      <c r="BG17" s="61"/>
+      <c r="BH17" s="61"/>
+      <c r="BI17" s="61"/>
+      <c r="BJ17" s="61"/>
+      <c r="BK17" s="61"/>
+      <c r="BL17" s="61"/>
+      <c r="BM17" s="61"/>
+      <c r="BN17" s="61"/>
+      <c r="BO17" s="61"/>
+      <c r="BP17" s="61"/>
+      <c r="BQ17" s="61"/>
+      <c r="BR17" s="61"/>
+      <c r="BS17" s="61"/>
+      <c r="BT17" s="61"/>
+      <c r="BU17" s="61"/>
+      <c r="BV17" s="61"/>
+      <c r="BW17" s="61"/>
+      <c r="BX17" s="61"/>
+      <c r="BY17" s="61"/>
+      <c r="BZ17" s="61"/>
+      <c r="CA17" s="61"/>
+      <c r="CB17" s="61"/>
+      <c r="CC17" s="61"/>
+      <c r="CD17" s="61"/>
+      <c r="CE17" s="61"/>
+      <c r="CF17" s="61"/>
+      <c r="CG17" s="61"/>
+      <c r="CH17" s="61"/>
+      <c r="CI17" s="61"/>
+      <c r="CJ17" s="61"/>
+      <c r="CK17" s="61"/>
+      <c r="CL17" s="61"/>
+      <c r="CM17" s="61"/>
+      <c r="CN17" s="61"/>
+      <c r="CO17" s="61"/>
+      <c r="CP17" s="61"/>
+      <c r="CQ17" s="61"/>
+      <c r="CR17" s="61"/>
+      <c r="CS17" s="61"/>
+      <c r="CT17" s="61"/>
+      <c r="CU17" s="61"/>
+      <c r="CV17" s="61"/>
+      <c r="CW17" s="61"/>
+      <c r="CX17" s="61"/>
+      <c r="CY17" s="61"/>
+      <c r="CZ17" s="61"/>
+      <c r="DA17" s="61"/>
+      <c r="DB17" s="61"/>
+      <c r="DC17" s="61"/>
+      <c r="DD17" s="61"/>
+      <c r="DE17" s="61"/>
+      <c r="DF17" s="61"/>
+      <c r="DG17" s="61"/>
+      <c r="DH17" s="61"/>
+      <c r="DI17" s="61"/>
+      <c r="DJ17" s="61"/>
+      <c r="DK17" s="61"/>
+      <c r="DL17" s="61"/>
+      <c r="DM17" s="61"/>
+      <c r="DN17" s="61"/>
+      <c r="DO17" s="61"/>
+      <c r="DP17" s="61"/>
+      <c r="DQ17" s="61"/>
+      <c r="DR17" s="61"/>
+      <c r="DS17" s="61"/>
+      <c r="DT17" s="61"/>
+      <c r="DU17" s="61"/>
+      <c r="DV17" s="61"/>
+      <c r="DW17" s="61"/>
+      <c r="DX17" s="61"/>
+      <c r="DY17" s="61"/>
+      <c r="DZ17" s="61"/>
+      <c r="EA17" s="61"/>
+      <c r="EB17" s="61"/>
+      <c r="EC17" s="61"/>
+      <c r="ED17" s="61"/>
+      <c r="EE17" s="61"/>
+      <c r="EF17" s="61"/>
+      <c r="EG17" s="61"/>
+      <c r="EH17" s="61"/>
+      <c r="EI17" s="61"/>
+      <c r="EJ17" s="61"/>
+      <c r="EK17" s="61"/>
+      <c r="EL17" s="61"/>
+      <c r="EM17" s="61"/>
+      <c r="EN17" s="61"/>
+      <c r="EO17" s="61"/>
+      <c r="EP17" s="61"/>
+      <c r="EQ17" s="61"/>
+      <c r="ER17" s="61"/>
+      <c r="ES17" s="61"/>
+      <c r="ET17" s="61"/>
+      <c r="EU17" s="61"/>
+      <c r="EV17" s="61"/>
+      <c r="EW17" s="61"/>
+      <c r="EX17" s="61"/>
+      <c r="EY17" s="61"/>
+      <c r="EZ17" s="61"/>
+      <c r="FA17" s="61"/>
+      <c r="FB17" s="61"/>
+      <c r="FC17" s="61"/>
+      <c r="FD17" s="61"/>
+      <c r="FE17" s="61"/>
+      <c r="FF17" s="61"/>
+      <c r="FG17" s="61"/>
+      <c r="FH17" s="61"/>
+      <c r="FI17" s="61"/>
+      <c r="FJ17" s="61"/>
+      <c r="FK17" s="61"/>
+      <c r="FL17" s="61"/>
+      <c r="FM17" s="61"/>
+      <c r="FN17" s="61"/>
+      <c r="FO17" s="61"/>
+      <c r="FP17" s="61"/>
+      <c r="FQ17" s="61"/>
+      <c r="FR17" s="61"/>
+      <c r="FS17" s="61"/>
+      <c r="FT17" s="61"/>
+      <c r="FU17" s="61"/>
+      <c r="FV17" s="61"/>
+      <c r="FW17" s="61"/>
+      <c r="FX17" s="61"/>
+      <c r="FY17" s="61"/>
+      <c r="FZ17" s="61"/>
+      <c r="GA17" s="61"/>
+      <c r="GB17" s="61"/>
+      <c r="GC17" s="61"/>
+      <c r="GD17" s="61"/>
+      <c r="GE17" s="61"/>
+      <c r="GF17" s="61"/>
+      <c r="GG17" s="61"/>
+      <c r="GH17" s="61"/>
+      <c r="GI17" s="61"/>
+      <c r="GJ17" s="61"/>
+      <c r="GK17" s="61"/>
+      <c r="GL17" s="61"/>
+      <c r="GM17" s="61"/>
+      <c r="GN17" s="61"/>
+      <c r="GO17" s="61"/>
+      <c r="GP17" s="61"/>
+      <c r="GQ17" s="61"/>
+      <c r="GR17" s="61"/>
+      <c r="GS17" s="61"/>
+      <c r="GT17" s="61"/>
+      <c r="GU17" s="61"/>
+      <c r="GV17" s="61"/>
+      <c r="GW17" s="61"/>
+      <c r="GX17" s="61"/>
+      <c r="GY17" s="61"/>
+      <c r="GZ17" s="61"/>
+      <c r="HA17" s="61"/>
+      <c r="HB17" s="61"/>
+      <c r="HC17" s="61"/>
+      <c r="HD17" s="61"/>
+      <c r="HE17" s="61"/>
+      <c r="HF17" s="61"/>
+      <c r="HG17" s="61"/>
+      <c r="HH17" s="61"/>
+      <c r="HI17" s="61"/>
+      <c r="HJ17" s="61"/>
+      <c r="HK17" s="61"/>
+      <c r="HL17" s="61"/>
+      <c r="HM17" s="61"/>
+      <c r="HN17" s="61"/>
+      <c r="HO17" s="61"/>
+      <c r="HP17" s="61"/>
+      <c r="HQ17" s="61"/>
+      <c r="HR17" s="61"/>
+      <c r="HS17" s="61"/>
+      <c r="HT17" s="61"/>
+      <c r="HU17" s="61"/>
+      <c r="HV17" s="61"/>
+      <c r="HW17" s="61"/>
+      <c r="HX17" s="61"/>
+      <c r="HY17" s="61"/>
+      <c r="HZ17" s="61"/>
+      <c r="IA17" s="61"/>
+      <c r="IB17" s="61"/>
+      <c r="IC17" s="61"/>
+      <c r="ID17" s="61"/>
+      <c r="IE17" s="61"/>
+      <c r="IF17" s="61"/>
+      <c r="IG17" s="61"/>
+      <c r="IH17" s="61"/>
+      <c r="II17" s="61"/>
+      <c r="IJ17" s="61"/>
+      <c r="IK17" s="61"/>
+      <c r="IL17" s="61"/>
+      <c r="IM17" s="61"/>
+      <c r="IN17" s="61"/>
+      <c r="IO17" s="61"/>
+      <c r="IP17" s="61"/>
+      <c r="IQ17" s="61"/>
+      <c r="IR17" s="61"/>
+      <c r="IS17" s="61"/>
+      <c r="IT17" s="61"/>
+      <c r="IU17" s="61"/>
+      <c r="IV17" s="61"/>
+    </row>
+    <row r="18" spans="1:256" s="71" customFormat="1" ht="144.6" customHeight="1">
+      <c r="A18" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B18" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="68"/>
+      <c r="Q18" s="68"/>
+      <c r="R18" s="68"/>
+      <c r="S18" s="68"/>
+      <c r="T18" s="68"/>
+      <c r="U18" s="68"/>
+      <c r="V18" s="68"/>
+      <c r="W18" s="68"/>
+      <c r="X18" s="68"/>
+      <c r="Y18" s="68"/>
+      <c r="Z18" s="68"/>
+      <c r="AA18" s="68"/>
+      <c r="AB18" s="69"/>
+      <c r="AC18" s="70"/>
+      <c r="AD18" s="70"/>
+      <c r="AE18" s="70"/>
+      <c r="AF18" s="70"/>
+      <c r="AG18" s="70"/>
+      <c r="AH18" s="70"/>
+      <c r="AI18" s="70"/>
+      <c r="AJ18" s="70"/>
+      <c r="AK18" s="70"/>
+      <c r="AL18" s="70"/>
+      <c r="AM18" s="70"/>
+      <c r="AN18" s="70"/>
+      <c r="AO18" s="70"/>
+      <c r="AP18" s="70"/>
+      <c r="AQ18" s="70"/>
+      <c r="AR18" s="70"/>
+      <c r="AS18" s="70"/>
+      <c r="AT18" s="70"/>
+      <c r="AU18" s="70"/>
+      <c r="AV18" s="70"/>
+      <c r="AW18" s="70"/>
+      <c r="AX18" s="70"/>
+      <c r="AY18" s="70"/>
+      <c r="AZ18" s="70"/>
+      <c r="BA18" s="70"/>
+      <c r="BB18" s="70"/>
+      <c r="BC18" s="70"/>
+      <c r="BD18" s="70"/>
+      <c r="BE18" s="70"/>
+      <c r="BF18" s="70"/>
+      <c r="BG18" s="70"/>
+      <c r="BH18" s="70"/>
+      <c r="BI18" s="70"/>
+      <c r="BJ18" s="70"/>
+      <c r="BK18" s="70"/>
+      <c r="BL18" s="70"/>
+      <c r="BM18" s="70"/>
+      <c r="BN18" s="70"/>
+      <c r="BO18" s="70"/>
+      <c r="BP18" s="70"/>
+      <c r="BQ18" s="70"/>
+      <c r="BR18" s="70"/>
+      <c r="BS18" s="70"/>
+      <c r="BT18" s="70"/>
+      <c r="BU18" s="70"/>
+      <c r="BV18" s="70"/>
+      <c r="BW18" s="70"/>
+      <c r="BX18" s="70"/>
+      <c r="BY18" s="70"/>
+      <c r="BZ18" s="70"/>
+      <c r="CA18" s="70"/>
+      <c r="CB18" s="70"/>
+      <c r="CC18" s="70"/>
+      <c r="CD18" s="70"/>
+      <c r="CE18" s="70"/>
+      <c r="CF18" s="70"/>
+      <c r="CG18" s="70"/>
+      <c r="CH18" s="70"/>
+      <c r="CI18" s="70"/>
+      <c r="CJ18" s="70"/>
+      <c r="CK18" s="70"/>
+      <c r="CL18" s="70"/>
+      <c r="CM18" s="70"/>
+      <c r="CN18" s="70"/>
+      <c r="CO18" s="70"/>
+      <c r="CP18" s="70"/>
+      <c r="CQ18" s="70"/>
+      <c r="CR18" s="70"/>
+      <c r="CS18" s="70"/>
+      <c r="CT18" s="70"/>
+      <c r="CU18" s="70"/>
+      <c r="CV18" s="70"/>
+      <c r="CW18" s="70"/>
+      <c r="CX18" s="70"/>
+      <c r="CY18" s="70"/>
+      <c r="CZ18" s="70"/>
+      <c r="DA18" s="70"/>
+      <c r="DB18" s="70"/>
+      <c r="DC18" s="70"/>
+      <c r="DD18" s="70"/>
+      <c r="DE18" s="70"/>
+      <c r="DF18" s="70"/>
+      <c r="DG18" s="70"/>
+      <c r="DH18" s="70"/>
+      <c r="DI18" s="70"/>
+      <c r="DJ18" s="70"/>
+      <c r="DK18" s="70"/>
+      <c r="DL18" s="70"/>
+      <c r="DM18" s="70"/>
+      <c r="DN18" s="70"/>
+      <c r="DO18" s="70"/>
+      <c r="DP18" s="70"/>
+      <c r="DQ18" s="70"/>
+      <c r="DR18" s="70"/>
+      <c r="DS18" s="70"/>
+      <c r="DT18" s="70"/>
+      <c r="DU18" s="70"/>
+      <c r="DV18" s="70"/>
+      <c r="DW18" s="70"/>
+      <c r="DX18" s="70"/>
+      <c r="DY18" s="70"/>
+      <c r="DZ18" s="70"/>
+      <c r="EA18" s="70"/>
+      <c r="EB18" s="70"/>
+      <c r="EC18" s="70"/>
+      <c r="ED18" s="70"/>
+      <c r="EE18" s="70"/>
+      <c r="EF18" s="70"/>
+      <c r="EG18" s="70"/>
+      <c r="EH18" s="70"/>
+      <c r="EI18" s="70"/>
+      <c r="EJ18" s="70"/>
+      <c r="EK18" s="70"/>
+      <c r="EL18" s="70"/>
+      <c r="EM18" s="70"/>
+      <c r="EN18" s="70"/>
+      <c r="EO18" s="70"/>
+      <c r="EP18" s="70"/>
+      <c r="EQ18" s="70"/>
+      <c r="ER18" s="70"/>
+      <c r="ES18" s="70"/>
+      <c r="ET18" s="70"/>
+      <c r="EU18" s="70"/>
+      <c r="EV18" s="70"/>
+      <c r="EW18" s="70"/>
+      <c r="EX18" s="70"/>
+      <c r="EY18" s="70"/>
+      <c r="EZ18" s="70"/>
+      <c r="FA18" s="70"/>
+      <c r="FB18" s="70"/>
+      <c r="FC18" s="70"/>
+      <c r="FD18" s="70"/>
+      <c r="FE18" s="70"/>
+      <c r="FF18" s="70"/>
+      <c r="FG18" s="70"/>
+      <c r="FH18" s="70"/>
+      <c r="FI18" s="70"/>
+      <c r="FJ18" s="70"/>
+      <c r="FK18" s="70"/>
+      <c r="FL18" s="70"/>
+      <c r="FM18" s="70"/>
+      <c r="FN18" s="70"/>
+      <c r="FO18" s="70"/>
+      <c r="FP18" s="70"/>
+      <c r="FQ18" s="70"/>
+      <c r="FR18" s="70"/>
+      <c r="FS18" s="70"/>
+      <c r="FT18" s="70"/>
+      <c r="FU18" s="70"/>
+      <c r="FV18" s="70"/>
+      <c r="FW18" s="70"/>
+      <c r="FX18" s="70"/>
+      <c r="FY18" s="70"/>
+      <c r="FZ18" s="70"/>
+      <c r="GA18" s="70"/>
+      <c r="GB18" s="70"/>
+      <c r="GC18" s="70"/>
+      <c r="GD18" s="70"/>
+      <c r="GE18" s="70"/>
+      <c r="GF18" s="70"/>
+      <c r="GG18" s="70"/>
+      <c r="GH18" s="70"/>
+      <c r="GI18" s="70"/>
+      <c r="GJ18" s="70"/>
+      <c r="GK18" s="70"/>
+      <c r="GL18" s="70"/>
+      <c r="GM18" s="70"/>
+      <c r="GN18" s="70"/>
+      <c r="GO18" s="70"/>
+      <c r="GP18" s="70"/>
+      <c r="GQ18" s="70"/>
+      <c r="GR18" s="70"/>
+      <c r="GS18" s="70"/>
+      <c r="GT18" s="70"/>
+      <c r="GU18" s="70"/>
+      <c r="GV18" s="70"/>
+      <c r="GW18" s="70"/>
+      <c r="GX18" s="70"/>
+      <c r="GY18" s="70"/>
+      <c r="GZ18" s="70"/>
+      <c r="HA18" s="70"/>
+      <c r="HB18" s="70"/>
+      <c r="HC18" s="70"/>
+      <c r="HD18" s="70"/>
+      <c r="HE18" s="70"/>
+      <c r="HF18" s="70"/>
+      <c r="HG18" s="70"/>
+      <c r="HH18" s="70"/>
+      <c r="HI18" s="70"/>
+      <c r="HJ18" s="70"/>
+      <c r="HK18" s="70"/>
+      <c r="HL18" s="70"/>
+      <c r="HM18" s="70"/>
+      <c r="HN18" s="70"/>
+      <c r="HO18" s="70"/>
+      <c r="HP18" s="70"/>
+      <c r="HQ18" s="70"/>
+      <c r="HR18" s="70"/>
+      <c r="HS18" s="70"/>
+      <c r="HT18" s="70"/>
+      <c r="HU18" s="70"/>
+      <c r="HV18" s="70"/>
+      <c r="HW18" s="70"/>
+      <c r="HX18" s="70"/>
+      <c r="HY18" s="70"/>
+      <c r="HZ18" s="70"/>
+      <c r="IA18" s="70"/>
+      <c r="IB18" s="70"/>
+      <c r="IC18" s="70"/>
+      <c r="ID18" s="70"/>
+      <c r="IE18" s="70"/>
+      <c r="IF18" s="70"/>
+      <c r="IG18" s="70"/>
+      <c r="IH18" s="70"/>
+      <c r="II18" s="70"/>
+      <c r="IJ18" s="70"/>
+      <c r="IK18" s="70"/>
+      <c r="IL18" s="70"/>
+      <c r="IM18" s="70"/>
+      <c r="IN18" s="70"/>
+      <c r="IO18" s="70"/>
+      <c r="IP18" s="70"/>
+      <c r="IQ18" s="70"/>
+      <c r="IR18" s="70"/>
+      <c r="IS18" s="70"/>
+      <c r="IT18" s="70"/>
+      <c r="IU18" s="70"/>
+      <c r="IV18" s="70"/>
+    </row>
+    <row r="19" spans="1:256" s="62" customFormat="1" ht="195.6" hidden="1" customHeight="1">
+      <c r="A19" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="59"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="59"/>
+      <c r="V19" s="59"/>
+      <c r="W19" s="59"/>
+      <c r="X19" s="59"/>
+      <c r="Y19" s="59"/>
+      <c r="Z19" s="59"/>
+      <c r="AA19" s="59"/>
+      <c r="AB19" s="60"/>
+      <c r="AC19" s="61"/>
+      <c r="AD19" s="61"/>
+      <c r="AE19" s="61"/>
+      <c r="AF19" s="61"/>
+      <c r="AG19" s="61"/>
+      <c r="AH19" s="61"/>
+      <c r="AI19" s="61"/>
+      <c r="AJ19" s="61"/>
+      <c r="AK19" s="61"/>
+      <c r="AL19" s="61"/>
+      <c r="AM19" s="61"/>
+      <c r="AN19" s="61"/>
+      <c r="AO19" s="61"/>
+      <c r="AP19" s="61"/>
+      <c r="AQ19" s="61"/>
+      <c r="AR19" s="61"/>
+      <c r="AS19" s="61"/>
+      <c r="AT19" s="61"/>
+      <c r="AU19" s="61"/>
+      <c r="AV19" s="61"/>
+      <c r="AW19" s="61"/>
+      <c r="AX19" s="61"/>
+      <c r="AY19" s="61"/>
+      <c r="AZ19" s="61"/>
+      <c r="BA19" s="61"/>
+      <c r="BB19" s="61"/>
+      <c r="BC19" s="61"/>
+      <c r="BD19" s="61"/>
+      <c r="BE19" s="61"/>
+      <c r="BF19" s="61"/>
+      <c r="BG19" s="61"/>
+      <c r="BH19" s="61"/>
+      <c r="BI19" s="61"/>
+      <c r="BJ19" s="61"/>
+      <c r="BK19" s="61"/>
+      <c r="BL19" s="61"/>
+      <c r="BM19" s="61"/>
+      <c r="BN19" s="61"/>
+      <c r="BO19" s="61"/>
+      <c r="BP19" s="61"/>
+      <c r="BQ19" s="61"/>
+      <c r="BR19" s="61"/>
+      <c r="BS19" s="61"/>
+      <c r="BT19" s="61"/>
+      <c r="BU19" s="61"/>
+      <c r="BV19" s="61"/>
+      <c r="BW19" s="61"/>
+      <c r="BX19" s="61"/>
+      <c r="BY19" s="61"/>
+      <c r="BZ19" s="61"/>
+      <c r="CA19" s="61"/>
+      <c r="CB19" s="61"/>
+      <c r="CC19" s="61"/>
+      <c r="CD19" s="61"/>
+      <c r="CE19" s="61"/>
+      <c r="CF19" s="61"/>
+      <c r="CG19" s="61"/>
+      <c r="CH19" s="61"/>
+      <c r="CI19" s="61"/>
+      <c r="CJ19" s="61"/>
+      <c r="CK19" s="61"/>
+      <c r="CL19" s="61"/>
+      <c r="CM19" s="61"/>
+      <c r="CN19" s="61"/>
+      <c r="CO19" s="61"/>
+      <c r="CP19" s="61"/>
+      <c r="CQ19" s="61"/>
+      <c r="CR19" s="61"/>
+      <c r="CS19" s="61"/>
+      <c r="CT19" s="61"/>
+      <c r="CU19" s="61"/>
+      <c r="CV19" s="61"/>
+      <c r="CW19" s="61"/>
+      <c r="CX19" s="61"/>
+      <c r="CY19" s="61"/>
+      <c r="CZ19" s="61"/>
+      <c r="DA19" s="61"/>
+      <c r="DB19" s="61"/>
+      <c r="DC19" s="61"/>
+      <c r="DD19" s="61"/>
+      <c r="DE19" s="61"/>
+      <c r="DF19" s="61"/>
+      <c r="DG19" s="61"/>
+      <c r="DH19" s="61"/>
+      <c r="DI19" s="61"/>
+      <c r="DJ19" s="61"/>
+      <c r="DK19" s="61"/>
+      <c r="DL19" s="61"/>
+      <c r="DM19" s="61"/>
+      <c r="DN19" s="61"/>
+      <c r="DO19" s="61"/>
+      <c r="DP19" s="61"/>
+      <c r="DQ19" s="61"/>
+      <c r="DR19" s="61"/>
+      <c r="DS19" s="61"/>
+      <c r="DT19" s="61"/>
+      <c r="DU19" s="61"/>
+      <c r="DV19" s="61"/>
+      <c r="DW19" s="61"/>
+      <c r="DX19" s="61"/>
+      <c r="DY19" s="61"/>
+      <c r="DZ19" s="61"/>
+      <c r="EA19" s="61"/>
+      <c r="EB19" s="61"/>
+      <c r="EC19" s="61"/>
+      <c r="ED19" s="61"/>
+      <c r="EE19" s="61"/>
+      <c r="EF19" s="61"/>
+      <c r="EG19" s="61"/>
+      <c r="EH19" s="61"/>
+      <c r="EI19" s="61"/>
+      <c r="EJ19" s="61"/>
+      <c r="EK19" s="61"/>
+      <c r="EL19" s="61"/>
+      <c r="EM19" s="61"/>
+      <c r="EN19" s="61"/>
+      <c r="EO19" s="61"/>
+      <c r="EP19" s="61"/>
+      <c r="EQ19" s="61"/>
+      <c r="ER19" s="61"/>
+      <c r="ES19" s="61"/>
+      <c r="ET19" s="61"/>
+      <c r="EU19" s="61"/>
+      <c r="EV19" s="61"/>
+      <c r="EW19" s="61"/>
+      <c r="EX19" s="61"/>
+      <c r="EY19" s="61"/>
+      <c r="EZ19" s="61"/>
+      <c r="FA19" s="61"/>
+      <c r="FB19" s="61"/>
+      <c r="FC19" s="61"/>
+      <c r="FD19" s="61"/>
+      <c r="FE19" s="61"/>
+      <c r="FF19" s="61"/>
+      <c r="FG19" s="61"/>
+      <c r="FH19" s="61"/>
+      <c r="FI19" s="61"/>
+      <c r="FJ19" s="61"/>
+      <c r="FK19" s="61"/>
+      <c r="FL19" s="61"/>
+      <c r="FM19" s="61"/>
+      <c r="FN19" s="61"/>
+      <c r="FO19" s="61"/>
+      <c r="FP19" s="61"/>
+      <c r="FQ19" s="61"/>
+      <c r="FR19" s="61"/>
+      <c r="FS19" s="61"/>
+      <c r="FT19" s="61"/>
+      <c r="FU19" s="61"/>
+      <c r="FV19" s="61"/>
+      <c r="FW19" s="61"/>
+      <c r="FX19" s="61"/>
+      <c r="FY19" s="61"/>
+      <c r="FZ19" s="61"/>
+      <c r="GA19" s="61"/>
+      <c r="GB19" s="61"/>
+      <c r="GC19" s="61"/>
+      <c r="GD19" s="61"/>
+      <c r="GE19" s="61"/>
+      <c r="GF19" s="61"/>
+      <c r="GG19" s="61"/>
+      <c r="GH19" s="61"/>
+      <c r="GI19" s="61"/>
+      <c r="GJ19" s="61"/>
+      <c r="GK19" s="61"/>
+      <c r="GL19" s="61"/>
+      <c r="GM19" s="61"/>
+      <c r="GN19" s="61"/>
+      <c r="GO19" s="61"/>
+      <c r="GP19" s="61"/>
+      <c r="GQ19" s="61"/>
+      <c r="GR19" s="61"/>
+      <c r="GS19" s="61"/>
+      <c r="GT19" s="61"/>
+      <c r="GU19" s="61"/>
+      <c r="GV19" s="61"/>
+      <c r="GW19" s="61"/>
+      <c r="GX19" s="61"/>
+      <c r="GY19" s="61"/>
+      <c r="GZ19" s="61"/>
+      <c r="HA19" s="61"/>
+      <c r="HB19" s="61"/>
+      <c r="HC19" s="61"/>
+      <c r="HD19" s="61"/>
+      <c r="HE19" s="61"/>
+      <c r="HF19" s="61"/>
+      <c r="HG19" s="61"/>
+      <c r="HH19" s="61"/>
+      <c r="HI19" s="61"/>
+      <c r="HJ19" s="61"/>
+      <c r="HK19" s="61"/>
+      <c r="HL19" s="61"/>
+      <c r="HM19" s="61"/>
+      <c r="HN19" s="61"/>
+      <c r="HO19" s="61"/>
+      <c r="HP19" s="61"/>
+      <c r="HQ19" s="61"/>
+      <c r="HR19" s="61"/>
+      <c r="HS19" s="61"/>
+      <c r="HT19" s="61"/>
+      <c r="HU19" s="61"/>
+      <c r="HV19" s="61"/>
+      <c r="HW19" s="61"/>
+      <c r="HX19" s="61"/>
+      <c r="HY19" s="61"/>
+      <c r="HZ19" s="61"/>
+      <c r="IA19" s="61"/>
+      <c r="IB19" s="61"/>
+      <c r="IC19" s="61"/>
+      <c r="ID19" s="61"/>
+      <c r="IE19" s="61"/>
+      <c r="IF19" s="61"/>
+      <c r="IG19" s="61"/>
+      <c r="IH19" s="61"/>
+      <c r="II19" s="61"/>
+      <c r="IJ19" s="61"/>
+      <c r="IK19" s="61"/>
+      <c r="IL19" s="61"/>
+      <c r="IM19" s="61"/>
+      <c r="IN19" s="61"/>
+      <c r="IO19" s="61"/>
+      <c r="IP19" s="61"/>
+      <c r="IQ19" s="61"/>
+      <c r="IR19" s="61"/>
+      <c r="IS19" s="61"/>
+      <c r="IT19" s="61"/>
+      <c r="IU19" s="61"/>
+      <c r="IV19" s="61"/>
+    </row>
+    <row r="20" spans="1:256" s="71" customFormat="1" ht="85.7" customHeight="1">
+      <c r="A20" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27" t="s">
-        <v>21</v>
+      <c r="C20" s="64" t="s">
+        <v>57</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="31"/>
-      <c r="AD17" s="31"/>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="31"/>
-      <c r="AH17" s="31"/>
-      <c r="AI17" s="31"/>
-      <c r="AJ17" s="31"/>
-      <c r="AK17" s="31"/>
-      <c r="AL17" s="31"/>
-      <c r="AM17" s="31"/>
-      <c r="AN17" s="31"/>
-      <c r="AO17" s="31"/>
-      <c r="AP17" s="31"/>
-      <c r="AQ17" s="31"/>
-      <c r="AR17" s="31"/>
-      <c r="AS17" s="31"/>
-      <c r="AT17" s="31"/>
-      <c r="AU17" s="31"/>
-      <c r="AV17" s="31"/>
-      <c r="AW17" s="31"/>
-      <c r="AX17" s="31"/>
-      <c r="AY17" s="31"/>
-      <c r="AZ17" s="31"/>
-      <c r="BA17" s="31"/>
-      <c r="BB17" s="31"/>
-      <c r="BC17" s="31"/>
-      <c r="BD17" s="31"/>
-      <c r="BE17" s="31"/>
-      <c r="BF17" s="31"/>
-      <c r="BG17" s="31"/>
-      <c r="BH17" s="31"/>
-      <c r="BI17" s="31"/>
-      <c r="BJ17" s="31"/>
-      <c r="BK17" s="31"/>
-      <c r="BL17" s="31"/>
-      <c r="BM17" s="31"/>
-      <c r="BN17" s="31"/>
-      <c r="BO17" s="31"/>
-      <c r="BP17" s="31"/>
-      <c r="BQ17" s="31"/>
-      <c r="BR17" s="31"/>
-      <c r="BS17" s="31"/>
-      <c r="BT17" s="31"/>
-      <c r="BU17" s="31"/>
-      <c r="BV17" s="31"/>
-      <c r="BW17" s="31"/>
-      <c r="BX17" s="31"/>
-      <c r="BY17" s="31"/>
-      <c r="BZ17" s="31"/>
-      <c r="CA17" s="31"/>
-      <c r="CB17" s="31"/>
-      <c r="CC17" s="31"/>
-      <c r="CD17" s="31"/>
-      <c r="CE17" s="31"/>
-      <c r="CF17" s="31"/>
-      <c r="CG17" s="31"/>
-      <c r="CH17" s="31"/>
-      <c r="CI17" s="31"/>
-      <c r="CJ17" s="31"/>
-      <c r="CK17" s="31"/>
-      <c r="CL17" s="31"/>
-      <c r="CM17" s="31"/>
-      <c r="CN17" s="31"/>
-      <c r="CO17" s="31"/>
-      <c r="CP17" s="31"/>
-      <c r="CQ17" s="31"/>
-      <c r="CR17" s="31"/>
-      <c r="CS17" s="31"/>
-      <c r="CT17" s="31"/>
-      <c r="CU17" s="31"/>
-      <c r="CV17" s="31"/>
-      <c r="CW17" s="31"/>
-      <c r="CX17" s="31"/>
-      <c r="CY17" s="31"/>
-      <c r="CZ17" s="31"/>
-      <c r="DA17" s="31"/>
-      <c r="DB17" s="31"/>
-      <c r="DC17" s="31"/>
-      <c r="DD17" s="31"/>
-      <c r="DE17" s="31"/>
-      <c r="DF17" s="31"/>
-      <c r="DG17" s="31"/>
-      <c r="DH17" s="31"/>
-      <c r="DI17" s="31"/>
-      <c r="DJ17" s="31"/>
-      <c r="DK17" s="31"/>
-      <c r="DL17" s="31"/>
-      <c r="DM17" s="31"/>
-      <c r="DN17" s="31"/>
-      <c r="DO17" s="31"/>
-      <c r="DP17" s="31"/>
-      <c r="DQ17" s="31"/>
-      <c r="DR17" s="31"/>
-      <c r="DS17" s="31"/>
-      <c r="DT17" s="31"/>
-      <c r="DU17" s="31"/>
-      <c r="DV17" s="31"/>
-      <c r="DW17" s="31"/>
-      <c r="DX17" s="31"/>
-      <c r="DY17" s="31"/>
-      <c r="DZ17" s="31"/>
-      <c r="EA17" s="31"/>
-      <c r="EB17" s="31"/>
-      <c r="EC17" s="31"/>
-      <c r="ED17" s="31"/>
-      <c r="EE17" s="31"/>
-      <c r="EF17" s="31"/>
-      <c r="EG17" s="31"/>
-      <c r="EH17" s="31"/>
-      <c r="EI17" s="31"/>
-      <c r="EJ17" s="31"/>
-      <c r="EK17" s="31"/>
-      <c r="EL17" s="31"/>
-      <c r="EM17" s="31"/>
-      <c r="EN17" s="31"/>
-      <c r="EO17" s="31"/>
-      <c r="EP17" s="31"/>
-      <c r="EQ17" s="31"/>
-      <c r="ER17" s="31"/>
-      <c r="ES17" s="31"/>
-      <c r="ET17" s="31"/>
-      <c r="EU17" s="31"/>
-      <c r="EV17" s="31"/>
-      <c r="EW17" s="31"/>
-      <c r="EX17" s="31"/>
-      <c r="EY17" s="31"/>
-      <c r="EZ17" s="31"/>
-      <c r="FA17" s="31"/>
-      <c r="FB17" s="31"/>
-      <c r="FC17" s="31"/>
-      <c r="FD17" s="31"/>
-      <c r="FE17" s="31"/>
-      <c r="FF17" s="31"/>
-      <c r="FG17" s="31"/>
-      <c r="FH17" s="31"/>
-      <c r="FI17" s="31"/>
-      <c r="FJ17" s="31"/>
-      <c r="FK17" s="31"/>
-      <c r="FL17" s="31"/>
-      <c r="FM17" s="31"/>
-      <c r="FN17" s="31"/>
-      <c r="FO17" s="31"/>
-      <c r="FP17" s="31"/>
-      <c r="FQ17" s="31"/>
-      <c r="FR17" s="31"/>
-      <c r="FS17" s="31"/>
-      <c r="FT17" s="31"/>
-      <c r="FU17" s="31"/>
-      <c r="FV17" s="31"/>
-      <c r="FW17" s="31"/>
-      <c r="FX17" s="31"/>
-      <c r="FY17" s="31"/>
-      <c r="FZ17" s="31"/>
-      <c r="GA17" s="31"/>
-      <c r="GB17" s="31"/>
-      <c r="GC17" s="31"/>
-      <c r="GD17" s="31"/>
-      <c r="GE17" s="31"/>
-      <c r="GF17" s="31"/>
-      <c r="GG17" s="31"/>
-      <c r="GH17" s="31"/>
-      <c r="GI17" s="31"/>
-      <c r="GJ17" s="31"/>
-      <c r="GK17" s="31"/>
-      <c r="GL17" s="31"/>
-      <c r="GM17" s="31"/>
-      <c r="GN17" s="31"/>
-      <c r="GO17" s="31"/>
-      <c r="GP17" s="31"/>
-      <c r="GQ17" s="31"/>
-      <c r="GR17" s="31"/>
-      <c r="GS17" s="31"/>
-      <c r="GT17" s="31"/>
-      <c r="GU17" s="31"/>
-      <c r="GV17" s="31"/>
-      <c r="GW17" s="31"/>
-      <c r="GX17" s="31"/>
-      <c r="GY17" s="31"/>
-      <c r="GZ17" s="31"/>
-      <c r="HA17" s="31"/>
-      <c r="HB17" s="31"/>
-      <c r="HC17" s="31"/>
-      <c r="HD17" s="31"/>
-      <c r="HE17" s="31"/>
-      <c r="HF17" s="31"/>
-      <c r="HG17" s="31"/>
-      <c r="HH17" s="31"/>
-      <c r="HI17" s="31"/>
-      <c r="HJ17" s="31"/>
-      <c r="HK17" s="31"/>
-      <c r="HL17" s="31"/>
-      <c r="HM17" s="31"/>
-      <c r="HN17" s="31"/>
-      <c r="HO17" s="31"/>
-      <c r="HP17" s="31"/>
-      <c r="HQ17" s="31"/>
-      <c r="HR17" s="31"/>
-      <c r="HS17" s="31"/>
-      <c r="HT17" s="31"/>
-      <c r="HU17" s="31"/>
-      <c r="HV17" s="31"/>
-      <c r="HW17" s="31"/>
-      <c r="HX17" s="31"/>
-      <c r="HY17" s="31"/>
-      <c r="HZ17" s="31"/>
-      <c r="IA17" s="31"/>
-      <c r="IB17" s="31"/>
-      <c r="IC17" s="31"/>
-      <c r="ID17" s="31"/>
-      <c r="IE17" s="31"/>
-      <c r="IF17" s="31"/>
-      <c r="IG17" s="31"/>
-      <c r="IH17" s="31"/>
-      <c r="II17" s="31"/>
-      <c r="IJ17" s="31"/>
-      <c r="IK17" s="31"/>
-      <c r="IL17" s="31"/>
-      <c r="IM17" s="31"/>
-      <c r="IN17" s="31"/>
-      <c r="IO17" s="31"/>
-      <c r="IP17" s="31"/>
-      <c r="IQ17" s="31"/>
-      <c r="IR17" s="31"/>
-      <c r="IS17" s="31"/>
-      <c r="IT17" s="31"/>
-      <c r="IU17" s="31"/>
-      <c r="IV17" s="31"/>
-    </row>
-    <row r="18" spans="1:256" ht="144.6" customHeight="1">
-      <c r="A18" s="50" t="s">
-        <v>42</v>
+      <c r="D20" s="64" t="s">
+        <v>20</v>
       </c>
-      <c r="B18" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="31"/>
-      <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-      <c r="AI18" s="31"/>
-      <c r="AJ18" s="31"/>
-      <c r="AK18" s="31"/>
-      <c r="AL18" s="31"/>
-      <c r="AM18" s="31"/>
-      <c r="AN18" s="31"/>
-      <c r="AO18" s="31"/>
-      <c r="AP18" s="31"/>
-      <c r="AQ18" s="31"/>
-      <c r="AR18" s="31"/>
-      <c r="AS18" s="31"/>
-      <c r="AT18" s="31"/>
-      <c r="AU18" s="31"/>
-      <c r="AV18" s="31"/>
-      <c r="AW18" s="31"/>
-      <c r="AX18" s="31"/>
-      <c r="AY18" s="31"/>
-      <c r="AZ18" s="31"/>
-      <c r="BA18" s="31"/>
-      <c r="BB18" s="31"/>
-      <c r="BC18" s="31"/>
-      <c r="BD18" s="31"/>
-      <c r="BE18" s="31"/>
-      <c r="BF18" s="31"/>
-      <c r="BG18" s="31"/>
-      <c r="BH18" s="31"/>
-      <c r="BI18" s="31"/>
-      <c r="BJ18" s="31"/>
-      <c r="BK18" s="31"/>
-      <c r="BL18" s="31"/>
-      <c r="BM18" s="31"/>
-      <c r="BN18" s="31"/>
-      <c r="BO18" s="31"/>
-      <c r="BP18" s="31"/>
-      <c r="BQ18" s="31"/>
-      <c r="BR18" s="31"/>
-      <c r="BS18" s="31"/>
-      <c r="BT18" s="31"/>
-      <c r="BU18" s="31"/>
-      <c r="BV18" s="31"/>
-      <c r="BW18" s="31"/>
-      <c r="BX18" s="31"/>
-      <c r="BY18" s="31"/>
-      <c r="BZ18" s="31"/>
-      <c r="CA18" s="31"/>
-      <c r="CB18" s="31"/>
-      <c r="CC18" s="31"/>
-      <c r="CD18" s="31"/>
-      <c r="CE18" s="31"/>
-      <c r="CF18" s="31"/>
-      <c r="CG18" s="31"/>
-      <c r="CH18" s="31"/>
-      <c r="CI18" s="31"/>
-      <c r="CJ18" s="31"/>
-      <c r="CK18" s="31"/>
-      <c r="CL18" s="31"/>
-      <c r="CM18" s="31"/>
-      <c r="CN18" s="31"/>
-      <c r="CO18" s="31"/>
-      <c r="CP18" s="31"/>
-      <c r="CQ18" s="31"/>
-      <c r="CR18" s="31"/>
-      <c r="CS18" s="31"/>
-      <c r="CT18" s="31"/>
-      <c r="CU18" s="31"/>
-      <c r="CV18" s="31"/>
-      <c r="CW18" s="31"/>
-      <c r="CX18" s="31"/>
-      <c r="CY18" s="31"/>
-      <c r="CZ18" s="31"/>
-      <c r="DA18" s="31"/>
-      <c r="DB18" s="31"/>
-      <c r="DC18" s="31"/>
-      <c r="DD18" s="31"/>
-      <c r="DE18" s="31"/>
-      <c r="DF18" s="31"/>
-      <c r="DG18" s="31"/>
-      <c r="DH18" s="31"/>
-      <c r="DI18" s="31"/>
-      <c r="DJ18" s="31"/>
-      <c r="DK18" s="31"/>
-      <c r="DL18" s="31"/>
-      <c r="DM18" s="31"/>
-      <c r="DN18" s="31"/>
-      <c r="DO18" s="31"/>
-      <c r="DP18" s="31"/>
-      <c r="DQ18" s="31"/>
-      <c r="DR18" s="31"/>
-      <c r="DS18" s="31"/>
-      <c r="DT18" s="31"/>
-      <c r="DU18" s="31"/>
-      <c r="DV18" s="31"/>
-      <c r="DW18" s="31"/>
-      <c r="DX18" s="31"/>
-      <c r="DY18" s="31"/>
-      <c r="DZ18" s="31"/>
-      <c r="EA18" s="31"/>
-      <c r="EB18" s="31"/>
-      <c r="EC18" s="31"/>
-      <c r="ED18" s="31"/>
-      <c r="EE18" s="31"/>
-      <c r="EF18" s="31"/>
-      <c r="EG18" s="31"/>
-      <c r="EH18" s="31"/>
-      <c r="EI18" s="31"/>
-      <c r="EJ18" s="31"/>
-      <c r="EK18" s="31"/>
-      <c r="EL18" s="31"/>
-      <c r="EM18" s="31"/>
-      <c r="EN18" s="31"/>
-      <c r="EO18" s="31"/>
-      <c r="EP18" s="31"/>
-      <c r="EQ18" s="31"/>
-      <c r="ER18" s="31"/>
-      <c r="ES18" s="31"/>
-      <c r="ET18" s="31"/>
-      <c r="EU18" s="31"/>
-      <c r="EV18" s="31"/>
-      <c r="EW18" s="31"/>
-      <c r="EX18" s="31"/>
-      <c r="EY18" s="31"/>
-      <c r="EZ18" s="31"/>
-      <c r="FA18" s="31"/>
-      <c r="FB18" s="31"/>
-      <c r="FC18" s="31"/>
-      <c r="FD18" s="31"/>
-      <c r="FE18" s="31"/>
-      <c r="FF18" s="31"/>
-      <c r="FG18" s="31"/>
-      <c r="FH18" s="31"/>
-      <c r="FI18" s="31"/>
-      <c r="FJ18" s="31"/>
-      <c r="FK18" s="31"/>
-      <c r="FL18" s="31"/>
-      <c r="FM18" s="31"/>
-      <c r="FN18" s="31"/>
-      <c r="FO18" s="31"/>
-      <c r="FP18" s="31"/>
-      <c r="FQ18" s="31"/>
-      <c r="FR18" s="31"/>
-      <c r="FS18" s="31"/>
-      <c r="FT18" s="31"/>
-      <c r="FU18" s="31"/>
-      <c r="FV18" s="31"/>
-      <c r="FW18" s="31"/>
-      <c r="FX18" s="31"/>
-      <c r="FY18" s="31"/>
-      <c r="FZ18" s="31"/>
-      <c r="GA18" s="31"/>
-      <c r="GB18" s="31"/>
-      <c r="GC18" s="31"/>
-      <c r="GD18" s="31"/>
-      <c r="GE18" s="31"/>
-      <c r="GF18" s="31"/>
-      <c r="GG18" s="31"/>
-      <c r="GH18" s="31"/>
-      <c r="GI18" s="31"/>
-      <c r="GJ18" s="31"/>
-      <c r="GK18" s="31"/>
-      <c r="GL18" s="31"/>
-      <c r="GM18" s="31"/>
-      <c r="GN18" s="31"/>
-      <c r="GO18" s="31"/>
-      <c r="GP18" s="31"/>
-      <c r="GQ18" s="31"/>
-      <c r="GR18" s="31"/>
-      <c r="GS18" s="31"/>
-      <c r="GT18" s="31"/>
-      <c r="GU18" s="31"/>
-      <c r="GV18" s="31"/>
-      <c r="GW18" s="31"/>
-      <c r="GX18" s="31"/>
-      <c r="GY18" s="31"/>
-      <c r="GZ18" s="31"/>
-      <c r="HA18" s="31"/>
-      <c r="HB18" s="31"/>
-      <c r="HC18" s="31"/>
-      <c r="HD18" s="31"/>
-      <c r="HE18" s="31"/>
-      <c r="HF18" s="31"/>
-      <c r="HG18" s="31"/>
-      <c r="HH18" s="31"/>
-      <c r="HI18" s="31"/>
-      <c r="HJ18" s="31"/>
-      <c r="HK18" s="31"/>
-      <c r="HL18" s="31"/>
-      <c r="HM18" s="31"/>
-      <c r="HN18" s="31"/>
-      <c r="HO18" s="31"/>
-      <c r="HP18" s="31"/>
-      <c r="HQ18" s="31"/>
-      <c r="HR18" s="31"/>
-      <c r="HS18" s="31"/>
-      <c r="HT18" s="31"/>
-      <c r="HU18" s="31"/>
-      <c r="HV18" s="31"/>
-      <c r="HW18" s="31"/>
-      <c r="HX18" s="31"/>
-      <c r="HY18" s="31"/>
-      <c r="HZ18" s="31"/>
-      <c r="IA18" s="31"/>
-      <c r="IB18" s="31"/>
-      <c r="IC18" s="31"/>
-      <c r="ID18" s="31"/>
-      <c r="IE18" s="31"/>
-      <c r="IF18" s="31"/>
-      <c r="IG18" s="31"/>
-      <c r="IH18" s="31"/>
-      <c r="II18" s="31"/>
-      <c r="IJ18" s="31"/>
-      <c r="IK18" s="31"/>
-      <c r="IL18" s="31"/>
-      <c r="IM18" s="31"/>
-      <c r="IN18" s="31"/>
-      <c r="IO18" s="31"/>
-      <c r="IP18" s="31"/>
-      <c r="IQ18" s="31"/>
-      <c r="IR18" s="31"/>
-      <c r="IS18" s="31"/>
-      <c r="IT18" s="31"/>
-      <c r="IU18" s="31"/>
-      <c r="IV18" s="31"/>
-    </row>
-    <row r="19" spans="1:256" ht="195.6" customHeight="1">
-      <c r="A19" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="7"/>
-    </row>
-    <row r="20" spans="1:256" ht="85.7" customHeight="1">
-      <c r="A20" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="7"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="68"/>
+      <c r="P20" s="68"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="68"/>
+      <c r="S20" s="68"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="68"/>
+      <c r="V20" s="68"/>
+      <c r="W20" s="68"/>
+      <c r="X20" s="68"/>
+      <c r="Y20" s="68"/>
+      <c r="Z20" s="68"/>
+      <c r="AA20" s="68"/>
+      <c r="AB20" s="69"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="70"/>
+      <c r="AF20" s="70"/>
+      <c r="AG20" s="70"/>
+      <c r="AH20" s="70"/>
+      <c r="AI20" s="70"/>
+      <c r="AJ20" s="70"/>
+      <c r="AK20" s="70"/>
+      <c r="AL20" s="70"/>
+      <c r="AM20" s="70"/>
+      <c r="AN20" s="70"/>
+      <c r="AO20" s="70"/>
+      <c r="AP20" s="70"/>
+      <c r="AQ20" s="70"/>
+      <c r="AR20" s="70"/>
+      <c r="AS20" s="70"/>
+      <c r="AT20" s="70"/>
+      <c r="AU20" s="70"/>
+      <c r="AV20" s="70"/>
+      <c r="AW20" s="70"/>
+      <c r="AX20" s="70"/>
+      <c r="AY20" s="70"/>
+      <c r="AZ20" s="70"/>
+      <c r="BA20" s="70"/>
+      <c r="BB20" s="70"/>
+      <c r="BC20" s="70"/>
+      <c r="BD20" s="70"/>
+      <c r="BE20" s="70"/>
+      <c r="BF20" s="70"/>
+      <c r="BG20" s="70"/>
+      <c r="BH20" s="70"/>
+      <c r="BI20" s="70"/>
+      <c r="BJ20" s="70"/>
+      <c r="BK20" s="70"/>
+      <c r="BL20" s="70"/>
+      <c r="BM20" s="70"/>
+      <c r="BN20" s="70"/>
+      <c r="BO20" s="70"/>
+      <c r="BP20" s="70"/>
+      <c r="BQ20" s="70"/>
+      <c r="BR20" s="70"/>
+      <c r="BS20" s="70"/>
+      <c r="BT20" s="70"/>
+      <c r="BU20" s="70"/>
+      <c r="BV20" s="70"/>
+      <c r="BW20" s="70"/>
+      <c r="BX20" s="70"/>
+      <c r="BY20" s="70"/>
+      <c r="BZ20" s="70"/>
+      <c r="CA20" s="70"/>
+      <c r="CB20" s="70"/>
+      <c r="CC20" s="70"/>
+      <c r="CD20" s="70"/>
+      <c r="CE20" s="70"/>
+      <c r="CF20" s="70"/>
+      <c r="CG20" s="70"/>
+      <c r="CH20" s="70"/>
+      <c r="CI20" s="70"/>
+      <c r="CJ20" s="70"/>
+      <c r="CK20" s="70"/>
+      <c r="CL20" s="70"/>
+      <c r="CM20" s="70"/>
+      <c r="CN20" s="70"/>
+      <c r="CO20" s="70"/>
+      <c r="CP20" s="70"/>
+      <c r="CQ20" s="70"/>
+      <c r="CR20" s="70"/>
+      <c r="CS20" s="70"/>
+      <c r="CT20" s="70"/>
+      <c r="CU20" s="70"/>
+      <c r="CV20" s="70"/>
+      <c r="CW20" s="70"/>
+      <c r="CX20" s="70"/>
+      <c r="CY20" s="70"/>
+      <c r="CZ20" s="70"/>
+      <c r="DA20" s="70"/>
+      <c r="DB20" s="70"/>
+      <c r="DC20" s="70"/>
+      <c r="DD20" s="70"/>
+      <c r="DE20" s="70"/>
+      <c r="DF20" s="70"/>
+      <c r="DG20" s="70"/>
+      <c r="DH20" s="70"/>
+      <c r="DI20" s="70"/>
+      <c r="DJ20" s="70"/>
+      <c r="DK20" s="70"/>
+      <c r="DL20" s="70"/>
+      <c r="DM20" s="70"/>
+      <c r="DN20" s="70"/>
+      <c r="DO20" s="70"/>
+      <c r="DP20" s="70"/>
+      <c r="DQ20" s="70"/>
+      <c r="DR20" s="70"/>
+      <c r="DS20" s="70"/>
+      <c r="DT20" s="70"/>
+      <c r="DU20" s="70"/>
+      <c r="DV20" s="70"/>
+      <c r="DW20" s="70"/>
+      <c r="DX20" s="70"/>
+      <c r="DY20" s="70"/>
+      <c r="DZ20" s="70"/>
+      <c r="EA20" s="70"/>
+      <c r="EB20" s="70"/>
+      <c r="EC20" s="70"/>
+      <c r="ED20" s="70"/>
+      <c r="EE20" s="70"/>
+      <c r="EF20" s="70"/>
+      <c r="EG20" s="70"/>
+      <c r="EH20" s="70"/>
+      <c r="EI20" s="70"/>
+      <c r="EJ20" s="70"/>
+      <c r="EK20" s="70"/>
+      <c r="EL20" s="70"/>
+      <c r="EM20" s="70"/>
+      <c r="EN20" s="70"/>
+      <c r="EO20" s="70"/>
+      <c r="EP20" s="70"/>
+      <c r="EQ20" s="70"/>
+      <c r="ER20" s="70"/>
+      <c r="ES20" s="70"/>
+      <c r="ET20" s="70"/>
+      <c r="EU20" s="70"/>
+      <c r="EV20" s="70"/>
+      <c r="EW20" s="70"/>
+      <c r="EX20" s="70"/>
+      <c r="EY20" s="70"/>
+      <c r="EZ20" s="70"/>
+      <c r="FA20" s="70"/>
+      <c r="FB20" s="70"/>
+      <c r="FC20" s="70"/>
+      <c r="FD20" s="70"/>
+      <c r="FE20" s="70"/>
+      <c r="FF20" s="70"/>
+      <c r="FG20" s="70"/>
+      <c r="FH20" s="70"/>
+      <c r="FI20" s="70"/>
+      <c r="FJ20" s="70"/>
+      <c r="FK20" s="70"/>
+      <c r="FL20" s="70"/>
+      <c r="FM20" s="70"/>
+      <c r="FN20" s="70"/>
+      <c r="FO20" s="70"/>
+      <c r="FP20" s="70"/>
+      <c r="FQ20" s="70"/>
+      <c r="FR20" s="70"/>
+      <c r="FS20" s="70"/>
+      <c r="FT20" s="70"/>
+      <c r="FU20" s="70"/>
+      <c r="FV20" s="70"/>
+      <c r="FW20" s="70"/>
+      <c r="FX20" s="70"/>
+      <c r="FY20" s="70"/>
+      <c r="FZ20" s="70"/>
+      <c r="GA20" s="70"/>
+      <c r="GB20" s="70"/>
+      <c r="GC20" s="70"/>
+      <c r="GD20" s="70"/>
+      <c r="GE20" s="70"/>
+      <c r="GF20" s="70"/>
+      <c r="GG20" s="70"/>
+      <c r="GH20" s="70"/>
+      <c r="GI20" s="70"/>
+      <c r="GJ20" s="70"/>
+      <c r="GK20" s="70"/>
+      <c r="GL20" s="70"/>
+      <c r="GM20" s="70"/>
+      <c r="GN20" s="70"/>
+      <c r="GO20" s="70"/>
+      <c r="GP20" s="70"/>
+      <c r="GQ20" s="70"/>
+      <c r="GR20" s="70"/>
+      <c r="GS20" s="70"/>
+      <c r="GT20" s="70"/>
+      <c r="GU20" s="70"/>
+      <c r="GV20" s="70"/>
+      <c r="GW20" s="70"/>
+      <c r="GX20" s="70"/>
+      <c r="GY20" s="70"/>
+      <c r="GZ20" s="70"/>
+      <c r="HA20" s="70"/>
+      <c r="HB20" s="70"/>
+      <c r="HC20" s="70"/>
+      <c r="HD20" s="70"/>
+      <c r="HE20" s="70"/>
+      <c r="HF20" s="70"/>
+      <c r="HG20" s="70"/>
+      <c r="HH20" s="70"/>
+      <c r="HI20" s="70"/>
+      <c r="HJ20" s="70"/>
+      <c r="HK20" s="70"/>
+      <c r="HL20" s="70"/>
+      <c r="HM20" s="70"/>
+      <c r="HN20" s="70"/>
+      <c r="HO20" s="70"/>
+      <c r="HP20" s="70"/>
+      <c r="HQ20" s="70"/>
+      <c r="HR20" s="70"/>
+      <c r="HS20" s="70"/>
+      <c r="HT20" s="70"/>
+      <c r="HU20" s="70"/>
+      <c r="HV20" s="70"/>
+      <c r="HW20" s="70"/>
+      <c r="HX20" s="70"/>
+      <c r="HY20" s="70"/>
+      <c r="HZ20" s="70"/>
+      <c r="IA20" s="70"/>
+      <c r="IB20" s="70"/>
+      <c r="IC20" s="70"/>
+      <c r="ID20" s="70"/>
+      <c r="IE20" s="70"/>
+      <c r="IF20" s="70"/>
+      <c r="IG20" s="70"/>
+      <c r="IH20" s="70"/>
+      <c r="II20" s="70"/>
+      <c r="IJ20" s="70"/>
+      <c r="IK20" s="70"/>
+      <c r="IL20" s="70"/>
+      <c r="IM20" s="70"/>
+      <c r="IN20" s="70"/>
+      <c r="IO20" s="70"/>
+      <c r="IP20" s="70"/>
+      <c r="IQ20" s="70"/>
+      <c r="IR20" s="70"/>
+      <c r="IS20" s="70"/>
+      <c r="IT20" s="70"/>
+      <c r="IU20" s="70"/>
+      <c r="IV20" s="70"/>
     </row>
     <row r="21" spans="1:256" ht="14.25" customHeight="1">
       <c r="A21" s="46"/>

</xml_diff>